<commit_message>
Create Service, Model folder. Modify package.json for SCSS compilation
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHICKEN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\DAI HOC\HK5\TTTN\iFoody\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="193">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -841,6 +841,15 @@
   </si>
   <si>
     <t>admin-store-list</t>
+  </si>
+  <si>
+    <t>models</t>
+  </si>
+  <si>
+    <t>favorite-product</t>
+  </si>
+  <si>
+    <t>favorite-store</t>
   </si>
 </sst>
 </file>
@@ -1490,66 +1499,6 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1559,6 +1508,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="% complete" xfId="12"/>
@@ -2688,41 +2697,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58" t="s">
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -2730,66 +2739,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="50" t="s">
+      <c r="Q2" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="52"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="68"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="59" t="s">
+      <c r="V2" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="61"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="60"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="62" t="s">
+      <c r="AA2" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="64"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="63"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="59" t="s">
+      <c r="AI2" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="60"/>
-      <c r="AP2" s="60"/>
+      <c r="AJ2" s="59"/>
+      <c r="AK2" s="59"/>
+      <c r="AL2" s="59"/>
+      <c r="AM2" s="59"/>
+      <c r="AN2" s="59"/>
+      <c r="AO2" s="59"/>
+      <c r="AP2" s="59"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="64" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -2816,12 +2825,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="56"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>
@@ -4696,11 +4705,6 @@
     <row r="31" spans="2:52" ht="30" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:AB1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
@@ -4710,6 +4714,11 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:AB1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AI2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="BA5:BO30">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -4881,10 +4890,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4893,12 +4902,12 @@
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="B1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:15">
       <c r="B2" t="s">
         <v>144</v>
       </c>
@@ -4906,220 +4915,238 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:15">
       <c r="B3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:15">
       <c r="B4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:15">
       <c r="B5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>149</v>
       </c>
       <c r="J11" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="N11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>150</v>
       </c>
       <c r="K12" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1">
-      <c r="G13" s="72"/>
+      <c r="O12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" thickBot="1">
+      <c r="G13" s="52"/>
       <c r="K13" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="B14" s="68" t="s">
+      <c r="O13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="B14" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="70"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="50"/>
       <c r="K14" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="B15" s="71"/>
-      <c r="C15" s="72" t="s">
+      <c r="O14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="B15" s="51"/>
+      <c r="C15" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="73"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
       <c r="K15" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="B16" s="71"/>
-      <c r="C16" s="72" t="s">
+      <c r="O15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="B16" s="51"/>
+      <c r="C16" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72" t="s">
+      <c r="D16" s="52"/>
+      <c r="E16" s="52" t="s">
         <v>184</v>
       </c>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="73"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="53"/>
       <c r="K16" t="s">
         <v>162</v>
       </c>
+      <c r="O16" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="71"/>
-      <c r="C17" s="72" t="s">
+      <c r="B17" s="51"/>
+      <c r="C17" s="52" t="s">
         <v>151</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53"/>
       <c r="K17" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="71"/>
-      <c r="C18" s="72" t="s">
+      <c r="B18" s="51"/>
+      <c r="C18" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="73"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="53"/>
       <c r="K18" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="73"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="53"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="73"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="53"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="71"/>
-      <c r="C21" s="72" t="s">
+      <c r="B21" s="51"/>
+      <c r="C21" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="73"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="73"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72" t="s">
+      <c r="B23" s="51"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="G23" s="72" t="s">
+      <c r="G23" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="H23" s="73"/>
+      <c r="H23" s="53"/>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72" t="s">
+      <c r="B24" s="51"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="73"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
     </row>
     <row r="25" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="76"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="56"/>
     </row>
     <row r="26" spans="2:11">
-      <c r="G26" s="72"/>
+      <c r="G26" s="52"/>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11">
-      <c r="B30" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="2:2">
@@ -5220,13 +5247,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -5234,66 +5261,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="50" t="s">
+      <c r="Q2" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="52"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="68"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="59" t="s">
+      <c r="V2" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="61"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="60"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="62" t="s">
+      <c r="AA2" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="64"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="63"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="59" t="s">
+      <c r="AI2" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="60"/>
-      <c r="AP2" s="60"/>
+      <c r="AJ2" s="59"/>
+      <c r="AK2" s="59"/>
+      <c r="AL2" s="59"/>
+      <c r="AM2" s="59"/>
+      <c r="AN2" s="59"/>
+      <c r="AO2" s="59"/>
+      <c r="AP2" s="59"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="67" t="s">
+      <c r="F3" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="74" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -5320,12 +5347,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="56"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Structure Folder and Module
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,28 +18,29 @@
     <sheet name="Project Planner" sheetId="4" r:id="rId4"/>
     <sheet name="Note Teacher" sheetId="7" r:id="rId5"/>
     <sheet name="Note Project" sheetId="8" r:id="rId6"/>
-    <sheet name="Project Planner (sample)" sheetId="5" state="hidden" r:id="rId7"/>
+    <sheet name="Note Tuấn" sheetId="9" r:id="rId7"/>
+    <sheet name="Project Planner (sample)" sheetId="5" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Actual" localSheetId="6">('Project Planner (sample)'!PeriodInActual*('Project Planner (sample)'!$E1&gt;0))*'Project Planner (sample)'!PeriodInPlan</definedName>
+    <definedName name="Actual" localSheetId="7">('Project Planner (sample)'!PeriodInActual*('Project Planner (sample)'!$E1&gt;0))*'Project Planner (sample)'!PeriodInPlan</definedName>
     <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
-    <definedName name="ActualBeyond" localSheetId="6">'Project Planner (sample)'!PeriodInActual*('Project Planner (sample)'!$E1&gt;0)</definedName>
+    <definedName name="ActualBeyond" localSheetId="7">'Project Planner (sample)'!PeriodInActual*('Project Planner (sample)'!$E1&gt;0)</definedName>
     <definedName name="ActualBeyond">PeriodInActual*('Project Planner'!$E1&gt;0)</definedName>
-    <definedName name="PercentComplete" localSheetId="6">'Project Planner (sample)'!PercentCompleteBeyond*'Project Planner (sample)'!PeriodInPlan</definedName>
+    <definedName name="PercentComplete" localSheetId="7">'Project Planner (sample)'!PercentCompleteBeyond*'Project Planner (sample)'!PeriodInPlan</definedName>
     <definedName name="PercentComplete">PercentCompleteBeyond*PeriodInPlan</definedName>
-    <definedName name="PercentCompleteBeyond" localSheetId="6">('Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$E1,'Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1)*('Project Planner (sample)'!$E1&gt;0))*(('Project Planner (sample)'!A$4&lt;(INT('Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1*'Project Planner (sample)'!$G1)))+('Project Planner (sample)'!A$4='Project Planner (sample)'!$E1))*('Project Planner (sample)'!$G1&gt;0)</definedName>
+    <definedName name="PercentCompleteBeyond" localSheetId="7">('Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$E1,'Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1)*('Project Planner (sample)'!$E1&gt;0))*(('Project Planner (sample)'!A$4&lt;(INT('Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1*'Project Planner (sample)'!$G1)))+('Project Planner (sample)'!A$4='Project Planner (sample)'!$E1))*('Project Planner (sample)'!$G1&gt;0)</definedName>
     <definedName name="PercentCompleteBeyond">('Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1)*('Project Planner'!$E1&gt;0))*(('Project Planner'!A$4&lt;(INT('Project Planner'!$E1+'Project Planner'!$F1*'Project Planner'!$G1)))+('Project Planner'!A$4='Project Planner'!$E1))*('Project Planner'!$G1&gt;0)</definedName>
-    <definedName name="period_selected" localSheetId="6">'Project Planner (sample)'!$H$2</definedName>
+    <definedName name="period_selected" localSheetId="7">'Project Planner (sample)'!$H$2</definedName>
     <definedName name="period_selected">'Project Planner'!$H$2</definedName>
-    <definedName name="PeriodInActual" localSheetId="6">'Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$E1,'Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1-1)</definedName>
+    <definedName name="PeriodInActual" localSheetId="7">'Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$E1,'Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1-1)</definedName>
     <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1-1)</definedName>
-    <definedName name="PeriodInPlan" localSheetId="6">'Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$C1,'Project Planner (sample)'!$C1+'Project Planner (sample)'!$D1-1)</definedName>
+    <definedName name="PeriodInPlan" localSheetId="7">'Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$C1,'Project Planner (sample)'!$C1+'Project Planner (sample)'!$D1-1)</definedName>
     <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$C1,'Project Planner'!$C1+'Project Planner'!$D1-1)</definedName>
-    <definedName name="Plan" localSheetId="6">'Project Planner (sample)'!PeriodInPlan*('Project Planner (sample)'!$C1&gt;0)</definedName>
+    <definedName name="Plan" localSheetId="7">'Project Planner (sample)'!PeriodInPlan*('Project Planner (sample)'!$C1&gt;0)</definedName>
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Project Planner'!$3:$4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'Project Planner (sample)'!$3:$4</definedName>
-    <definedName name="TitleRegion..BO60" localSheetId="6">'Project Planner (sample)'!$B$3:$B$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'Project Planner (sample)'!$3:$4</definedName>
+    <definedName name="TitleRegion..BO60" localSheetId="7">'Project Planner (sample)'!$B$3:$B$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="243">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -726,9 +727,6 @@
     <t>Home</t>
   </si>
   <si>
-    <t>bs-dropdown</t>
-  </si>
-  <si>
     <t>bs-navbar</t>
   </si>
   <si>
@@ -744,24 +742,9 @@
     <t>product-item</t>
   </si>
   <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>auth</t>
-  </si>
-  <si>
-    <t>auth-guard</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>slider</t>
   </si>
   <si>
@@ -780,9 +763,6 @@
     <t>store-profile</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>admin-profile</t>
   </si>
   <si>
@@ -795,15 +775,6 @@
     <t>sign-up</t>
   </si>
   <si>
-    <t>password-change</t>
-  </si>
-  <si>
-    <t>password-reset</t>
-  </si>
-  <si>
-    <t>password-forgot</t>
-  </si>
-  <si>
     <t>store-open</t>
   </si>
   <si>
@@ -837,26 +808,206 @@
     <t>product-list</t>
   </si>
   <si>
-    <t>admin-user-list</t>
-  </si>
-  <si>
-    <t>admin-store-list</t>
-  </si>
-  <si>
     <t>models</t>
   </si>
   <si>
-    <t>favorite-product</t>
-  </si>
-  <si>
-    <t>favorite-store</t>
+    <t>Cài SCSS</t>
+  </si>
+  <si>
+    <t>SCSS là extension của CSS3 nên cái ji valid trong CSS3 đều valid trong SCSS.  SASS thì có syntax thụt đầu dòng cho từng property, cũ hơn SCSS.</t>
+  </si>
+  <si>
+    <t>Công việc: mở file Angular-cli.json thay đổi styleExt thành .scss   và đổi đường dẫn style sang file scss</t>
+  </si>
+  <si>
+    <t>Angular-CLI  tự động biên dịch SCSS, SASS, LESS file thành CSS nên ko cần cài thêm compiler khác (như Node_SASS)</t>
+  </si>
+  <si>
+    <t>Chú ý: file css tự đóng gói thành file JS nên muốn xem css phải chạy "ng build -prod" thay vì "ng build" hoặc câu lệnh khác</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>assets</t>
+  </si>
+  <si>
+    <t>environment</t>
+  </si>
+  <si>
+    <t>components</t>
+  </si>
+  <si>
+    <t>services</t>
+  </si>
+  <si>
+    <t>user.service</t>
+  </si>
+  <si>
+    <t>product.service</t>
+  </si>
+  <si>
+    <t>auth.service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user </t>
+  </si>
+  <si>
+    <t xml:space="preserve">product </t>
+  </si>
+  <si>
+    <t>store.service</t>
+  </si>
+  <si>
+    <t>shared (module)</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>Membership (module)</t>
+  </si>
+  <si>
+    <t>Core (module)</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>signup</t>
+  </si>
+  <si>
+    <t>change-password</t>
+  </si>
+  <si>
+    <t>reset-password</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>privacy</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>bs-breadcrumb</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>(kèm sao và số lượt đánh giá)</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>font</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>Admin (module)</t>
+  </si>
+  <si>
+    <t>admin-auth.service</t>
+  </si>
+  <si>
+    <t>forgot-password</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>admin-user</t>
+  </si>
+  <si>
+    <t>admin-store</t>
+  </si>
+  <si>
+    <t>admin-product</t>
+  </si>
+  <si>
+    <t>membership.service</t>
+  </si>
+  <si>
+    <t>Searching (module)</t>
+  </si>
+  <si>
+    <t>search-result</t>
+  </si>
+  <si>
+    <t>Uploading (module)</t>
+  </si>
+  <si>
+    <t>product-statistic</t>
+  </si>
+  <si>
+    <t>user-statistic</t>
+  </si>
+  <si>
+    <t>store-statistic</t>
+  </si>
+  <si>
+    <t>Có thể sử dụng lại ở các trang khác</t>
+  </si>
+  <si>
+    <t>Thuộc về ứng dụng</t>
+  </si>
+  <si>
+    <t>Structure iFoody  (chia theo functionallity)</t>
+  </si>
+  <si>
+    <t>Các chức năng liên quan đến member</t>
+  </si>
+  <si>
+    <t>Chú ý:</t>
+  </si>
+  <si>
+    <t>Tuấn</t>
+  </si>
+  <si>
+    <t>Phượng</t>
+  </si>
+  <si>
+    <t>Tạo module</t>
+  </si>
+  <si>
+    <t>ví dụ:       ng  g  m  shared    (tự động tạo file module trong folder shared được tạo trước đó)</t>
+  </si>
+  <si>
+    <t>bs-pagination</t>
+  </si>
+  <si>
+    <t>searchBar</t>
+  </si>
+  <si>
+    <t>Tạo Component, service, models</t>
+  </si>
+  <si>
+    <t>Tạo app.routing.ts</t>
+  </si>
+  <si>
+    <t>Route cho toàn bộ app (nếu đặt tất cả trong app.module.ts nhìn sẽ rất rối)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="32">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1084,6 +1235,22 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Roboto Mono"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1374,7 +1541,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1508,6 +1675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1567,6 +1735,19 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -2697,41 +2878,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57" t="s">
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -2739,66 +2920,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="66" t="s">
+      <c r="K2" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="69"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="66" t="s">
+      <c r="Q2" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="68"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="69"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="58" t="s">
+      <c r="V2" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="61"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="61" t="s">
+      <c r="AA2" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="64"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="58" t="s">
+      <c r="AI2" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="59"/>
-      <c r="AK2" s="59"/>
-      <c r="AL2" s="59"/>
-      <c r="AM2" s="59"/>
-      <c r="AN2" s="59"/>
-      <c r="AO2" s="59"/>
-      <c r="AP2" s="59"/>
+      <c r="AJ2" s="60"/>
+      <c r="AK2" s="60"/>
+      <c r="AL2" s="60"/>
+      <c r="AM2" s="60"/>
+      <c r="AN2" s="60"/>
+      <c r="AO2" s="60"/>
+      <c r="AP2" s="60"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="64" t="s">
+      <c r="G3" s="65" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -2825,12 +3006,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="72"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>
@@ -4890,323 +5071,774 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A2:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="2" spans="1:20">
+      <c r="A2" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="N2" s="57"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="57" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="B4" s="57" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="B5" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" s="81" t="s">
+        <v>229</v>
+      </c>
+      <c r="M5" s="57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="B6" s="80"/>
+      <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="M6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" thickBot="1">
+      <c r="B7" s="80"/>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
+      <c r="S7" s="52"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="B8" s="80"/>
+      <c r="E8" t="s">
+        <v>209</v>
+      </c>
+      <c r="N8" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="50"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="B9" s="80"/>
+      <c r="E9" t="s">
+        <v>238</v>
+      </c>
+      <c r="N9" s="51"/>
+      <c r="O9" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="53"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="B10" s="80"/>
+      <c r="D10" t="s">
+        <v>189</v>
+      </c>
+      <c r="N10" s="51"/>
+      <c r="O10" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="R10" s="52"/>
+      <c r="S10" s="52"/>
+      <c r="T10" s="53"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="B11" s="80"/>
+      <c r="E11" t="s">
+        <v>190</v>
+      </c>
+      <c r="N11" s="51"/>
+      <c r="O11" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
+      <c r="T11" s="53"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="B12" s="80"/>
+      <c r="E12" t="s">
+        <v>191</v>
+      </c>
+      <c r="N12" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="53"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="B13" s="80"/>
+      <c r="E13" t="s">
+        <v>195</v>
+      </c>
+      <c r="N13" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="52"/>
+      <c r="T13" s="53"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="B14" s="80"/>
+      <c r="E14" t="s">
+        <v>192</v>
+      </c>
+      <c r="N14" s="51"/>
+      <c r="O14" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="53"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="B15" s="80"/>
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="N15" s="51"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="52"/>
+      <c r="T15" s="53"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="B16" s="80"/>
+      <c r="E16" t="s">
+        <v>193</v>
+      </c>
+      <c r="N16" s="51"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="S16" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="T16" s="53"/>
+    </row>
+    <row r="17" spans="2:20">
+      <c r="B17" s="80"/>
+      <c r="E17" t="s">
+        <v>194</v>
+      </c>
+      <c r="N17" s="51"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
+      <c r="S17" s="52"/>
+      <c r="T17" s="53"/>
+    </row>
+    <row r="18" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B18" s="80"/>
+      <c r="E18" t="s">
+        <v>169</v>
+      </c>
+      <c r="N18" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="56"/>
+    </row>
+    <row r="19" spans="2:20">
+      <c r="B19" s="80"/>
+      <c r="E19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20">
+      <c r="B20" s="82" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>200</v>
+      </c>
+      <c r="H20" s="81" t="s">
+        <v>230</v>
+      </c>
+      <c r="S20" s="52"/>
+    </row>
+    <row r="21" spans="2:20">
+      <c r="B21" s="80"/>
+      <c r="D21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20">
+      <c r="B22" s="80"/>
+      <c r="E22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20">
+      <c r="B23" s="80"/>
+      <c r="E23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20">
+      <c r="B24" s="80"/>
+      <c r="E24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20">
+      <c r="B25" s="80"/>
+      <c r="E25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20">
+      <c r="B26" s="80"/>
+      <c r="E26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20">
+      <c r="B27" s="80"/>
+      <c r="E27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20">
+      <c r="B28" s="80"/>
+      <c r="E28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20">
+      <c r="B29" s="80"/>
+      <c r="E29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20">
+      <c r="B30" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="H30" s="81" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20">
+      <c r="B31" s="80"/>
+      <c r="D31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20">
+      <c r="B32" s="80"/>
+      <c r="E32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="80"/>
+      <c r="E33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="80"/>
+      <c r="E34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="80"/>
+      <c r="E35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="80"/>
+      <c r="E36" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="80"/>
+      <c r="E37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="80"/>
+      <c r="E38" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="80"/>
+      <c r="E39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="80"/>
+      <c r="E40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="80"/>
+      <c r="E41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="80"/>
+      <c r="D42" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="80"/>
+      <c r="E43" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="82" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="80"/>
+      <c r="D45" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" s="80"/>
+      <c r="E46" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="80"/>
+      <c r="E47" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" s="80"/>
+      <c r="E48" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="80"/>
+      <c r="E49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="80"/>
+      <c r="D50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="80"/>
+      <c r="E51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="80"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="57" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="80"/>
+      <c r="D54" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="80"/>
+      <c r="E55" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="80"/>
+      <c r="E56" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="80"/>
+      <c r="E57" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="80"/>
+      <c r="E58" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="80"/>
+      <c r="E59" t="s">
+        <v>210</v>
+      </c>
+      <c r="H59" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" s="80"/>
+      <c r="E60" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="80"/>
+      <c r="E61" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="80"/>
+      <c r="E62" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="80"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="82" t="s">
+        <v>235</v>
+      </c>
+      <c r="C64" s="57" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" s="79"/>
+      <c r="D65" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="79"/>
+      <c r="E66" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="79"/>
+      <c r="E67" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="79"/>
+      <c r="E68" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="79"/>
+      <c r="E69" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" s="79"/>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="78" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" s="79"/>
+      <c r="C72" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="B73" s="79"/>
+      <c r="C73" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="B74" s="79"/>
+      <c r="C74" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75" s="79"/>
+    </row>
+    <row r="76" spans="2:5">
+      <c r="B76" s="78" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="79"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="57" t="s">
+        <v>233</v>
+      </c>
       <c r="B1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="B2" t="s">
         <v>144</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="81" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="B3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="81" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="F4" s="81" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="F5" s="81" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="F6" s="81" t="s">
+        <v>183</v>
+      </c>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="B7" t="s">
+        <v>236</v>
+      </c>
+      <c r="F7" s="81" t="s">
+        <v>237</v>
+      </c>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="B8" t="s">
+        <v>240</v>
+      </c>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="81" t="s">
+        <v>242</v>
+      </c>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="81"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="B15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="B4" t="s">
+    <row r="16" spans="1:16">
+      <c r="B16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
-      <c r="B5" t="s">
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>149</v>
-      </c>
-      <c r="J11" t="s">
-        <v>157</v>
-      </c>
-      <c r="N11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>150</v>
-      </c>
-      <c r="K12" t="s">
-        <v>158</v>
-      </c>
-      <c r="O12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1">
-      <c r="G13" s="52"/>
-      <c r="K13" t="s">
-        <v>159</v>
-      </c>
-      <c r="O13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="B14" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="50"/>
-      <c r="K14" t="s">
-        <v>160</v>
-      </c>
-      <c r="O14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="B15" s="51"/>
-      <c r="C15" s="52" t="s">
-        <v>181</v>
-      </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="53"/>
-      <c r="K15" t="s">
-        <v>161</v>
-      </c>
-      <c r="O15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="B16" s="51"/>
-      <c r="C16" s="52" t="s">
-        <v>153</v>
-      </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52" t="s">
-        <v>184</v>
-      </c>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53"/>
-      <c r="K16" t="s">
-        <v>162</v>
-      </c>
-      <c r="O16" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11">
-      <c r="B17" s="51"/>
-      <c r="C17" s="52" t="s">
-        <v>151</v>
-      </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53"/>
-      <c r="K17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11">
-      <c r="B18" s="51"/>
-      <c r="C18" s="52" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53"/>
-      <c r="K18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11">
-      <c r="B19" s="51" t="s">
-        <v>163</v>
-      </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="53"/>
-    </row>
-    <row r="20" spans="2:11">
-      <c r="B20" s="51" t="s">
-        <v>185</v>
-      </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
-    </row>
-    <row r="21" spans="2:11">
-      <c r="B21" s="51"/>
-      <c r="C21" s="52" t="s">
-        <v>186</v>
-      </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="53"/>
-    </row>
-    <row r="22" spans="2:11">
-      <c r="B22" s="51"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52" t="s">
-        <v>187</v>
-      </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="53"/>
-    </row>
-    <row r="23" spans="2:11">
-      <c r="B23" s="51"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="G23" s="52" t="s">
-        <v>183</v>
-      </c>
-      <c r="H23" s="53"/>
-    </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52" t="s">
-        <v>171</v>
-      </c>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="53"/>
-    </row>
-    <row r="25" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B25" s="54" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="56"/>
-    </row>
-    <row r="26" spans="2:11">
-      <c r="G26" s="52"/>
-    </row>
-    <row r="27" spans="2:11">
-      <c r="B27" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11">
-      <c r="B28" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11">
-      <c r="B29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11">
-      <c r="B31" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11">
-      <c r="B32" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -5214,7 +5846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
@@ -5247,13 +5879,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -5261,66 +5893,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="66" t="s">
+      <c r="K2" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="69"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="66" t="s">
+      <c r="Q2" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="68"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="69"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="58" t="s">
+      <c r="V2" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="61"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="61" t="s">
+      <c r="AA2" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="64"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="58" t="s">
+      <c r="AI2" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="59"/>
-      <c r="AK2" s="59"/>
-      <c r="AL2" s="59"/>
-      <c r="AM2" s="59"/>
-      <c r="AN2" s="59"/>
-      <c r="AO2" s="59"/>
-      <c r="AP2" s="59"/>
+      <c r="AJ2" s="60"/>
+      <c r="AK2" s="60"/>
+      <c r="AL2" s="60"/>
+      <c r="AM2" s="60"/>
+      <c r="AN2" s="60"/>
+      <c r="AO2" s="60"/>
+      <c r="AP2" s="60"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="75" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -5347,12 +5979,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="72"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update Configuration for app.routing.ts Modifying ts.lint.json , app.module.ts Add some new component.
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -721,9 +721,6 @@
     <t>List các section item để chú ý</t>
   </si>
   <si>
-    <t>Components</t>
-  </si>
-  <si>
     <t>Home</t>
   </si>
   <si>
@@ -1001,6 +998,9 @@
   </si>
   <si>
     <t>Route cho toàn bộ app (nếu đặt tất cả trong app.module.ts nhìn sẽ rất rối)</t>
+  </si>
+  <si>
+    <t>Components (outdated)</t>
   </si>
 </sst>
 </file>
@@ -1676,66 +1676,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1748,6 +1688,66 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -2878,41 +2878,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58" t="s">
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="73"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -2920,66 +2920,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="67" t="s">
+      <c r="K2" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="69"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="67"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="67" t="s">
+      <c r="Q2" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="69"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="67"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="59" t="s">
+      <c r="V2" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="61"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="76"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="62" t="s">
+      <c r="AA2" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="64"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="79"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="59" t="s">
+      <c r="AI2" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="60"/>
-      <c r="AP2" s="60"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="74" t="s">
+      <c r="F3" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="63" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -3006,12 +3006,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="73"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>
@@ -4886,6 +4886,11 @@
     <row r="31" spans="2:52" ht="30" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:AB1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
@@ -4895,11 +4900,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:AB1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AI2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="BA5:BO30">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -5073,8 +5073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T81"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5086,57 +5086,57 @@
   <sheetData>
     <row r="2" spans="1:20">
       <c r="A2" s="57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N2" s="57"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="57" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="B4" s="57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="B5" s="82" t="s">
-        <v>234</v>
+      <c r="B5" s="62" t="s">
+        <v>233</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>196</v>
-      </c>
-      <c r="H5" s="81" t="s">
-        <v>229</v>
+        <v>195</v>
+      </c>
+      <c r="H5" s="61" t="s">
+        <v>228</v>
       </c>
       <c r="M5" s="57" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="B6" s="60"/>
+      <c r="D6" t="s">
+        <v>187</v>
+      </c>
+      <c r="M6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
-      <c r="B6" s="80"/>
-      <c r="D6" t="s">
-        <v>188</v>
-      </c>
-      <c r="M6" t="s">
+    <row r="7" spans="1:20" ht="15.75" thickBot="1">
+      <c r="B7" s="60"/>
+      <c r="E7" t="s">
+        <v>154</v>
+      </c>
+      <c r="S7" s="52"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="B8" s="60"/>
+      <c r="E8" t="s">
+        <v>208</v>
+      </c>
+      <c r="N8" s="48" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1">
-      <c r="B7" s="80"/>
-      <c r="E7" t="s">
-        <v>155</v>
-      </c>
-      <c r="S7" s="52"/>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="B8" s="80"/>
-      <c r="E8" t="s">
-        <v>209</v>
-      </c>
-      <c r="N8" s="48" t="s">
-        <v>151</v>
       </c>
       <c r="O8" s="49"/>
       <c r="P8" s="49"/>
@@ -5146,13 +5146,13 @@
       <c r="T8" s="50"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="B9" s="80"/>
+      <c r="B9" s="60"/>
       <c r="E9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N9" s="51"/>
       <c r="O9" s="52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P9" s="52"/>
       <c r="Q9" s="52"/>
@@ -5161,30 +5161,30 @@
       <c r="T9" s="53"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="B10" s="80"/>
+      <c r="B10" s="60"/>
       <c r="D10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N10" s="51"/>
       <c r="O10" s="52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P10" s="52"/>
       <c r="Q10" s="52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R10" s="52"/>
       <c r="S10" s="52"/>
       <c r="T10" s="53"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="B11" s="80"/>
+      <c r="B11" s="60"/>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N11" s="51"/>
       <c r="O11" s="52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P11" s="52"/>
       <c r="Q11" s="52"/>
@@ -5193,12 +5193,12 @@
       <c r="T11" s="53"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="B12" s="80"/>
+      <c r="B12" s="60"/>
       <c r="E12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N12" s="51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O12" s="52"/>
       <c r="P12" s="52"/>
@@ -5208,12 +5208,12 @@
       <c r="T12" s="53"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="B13" s="80"/>
+      <c r="B13" s="60"/>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N13" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O13" s="52"/>
       <c r="P13" s="52"/>
@@ -5223,13 +5223,13 @@
       <c r="T13" s="53"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="B14" s="80"/>
+      <c r="B14" s="60"/>
       <c r="E14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N14" s="51"/>
       <c r="O14" s="52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P14" s="52"/>
       <c r="Q14" s="52"/>
@@ -5238,14 +5238,14 @@
       <c r="T14" s="53"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="B15" s="80"/>
+      <c r="B15" s="60"/>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N15" s="51"/>
       <c r="O15" s="52"/>
       <c r="P15" s="52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q15" s="52"/>
       <c r="R15" s="52"/>
@@ -5253,31 +5253,31 @@
       <c r="T15" s="53"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="B16" s="80"/>
+      <c r="B16" s="60"/>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N16" s="51"/>
       <c r="O16" s="52"/>
       <c r="P16" s="52"/>
       <c r="Q16" s="52"/>
       <c r="R16" s="52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S16" s="52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T16" s="53"/>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="80"/>
+      <c r="B17" s="60"/>
       <c r="E17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N17" s="51"/>
       <c r="O17" s="52"/>
       <c r="P17" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q17" s="52"/>
       <c r="R17" s="52"/>
@@ -5285,12 +5285,12 @@
       <c r="T17" s="53"/>
     </row>
     <row r="18" spans="2:20" ht="15.75" thickBot="1">
-      <c r="B18" s="80"/>
+      <c r="B18" s="60"/>
       <c r="E18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N18" s="54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O18" s="55"/>
       <c r="P18" s="55"/>
@@ -5300,361 +5300,361 @@
       <c r="T18" s="56"/>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="80"/>
+      <c r="B19" s="60"/>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="82" t="s">
-        <v>235</v>
+      <c r="B20" s="62" t="s">
+        <v>234</v>
       </c>
       <c r="C20" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="H20" s="61" t="s">
+        <v>229</v>
+      </c>
+      <c r="S20" s="52"/>
+    </row>
+    <row r="21" spans="2:20">
+      <c r="B21" s="60"/>
+      <c r="D21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20">
+      <c r="B22" s="60"/>
+      <c r="E22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20">
+      <c r="B23" s="60"/>
+      <c r="E23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20">
+      <c r="B24" s="60"/>
+      <c r="E24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20">
+      <c r="B25" s="60"/>
+      <c r="E25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20">
+      <c r="B26" s="60"/>
+      <c r="E26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20">
+      <c r="B27" s="60"/>
+      <c r="E27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20">
+      <c r="B28" s="60"/>
+      <c r="E28" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20">
+      <c r="B29" s="60"/>
+      <c r="E29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20">
+      <c r="B30" s="62" t="s">
+        <v>233</v>
+      </c>
+      <c r="C30" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="H30" s="61" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20">
+      <c r="B31" s="60"/>
+      <c r="D31" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20">
+      <c r="B32" s="60"/>
+      <c r="E32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="60"/>
+      <c r="E33" t="s">
         <v>200</v>
       </c>
-      <c r="H20" s="81" t="s">
-        <v>230</v>
-      </c>
-      <c r="S20" s="52"/>
-    </row>
-    <row r="21" spans="2:20">
-      <c r="B21" s="80"/>
-      <c r="D21" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="22" spans="2:20">
-      <c r="B22" s="80"/>
-      <c r="E22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="2:20">
-      <c r="B23" s="80"/>
-      <c r="E23" t="s">
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="60"/>
+      <c r="E34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="60"/>
+      <c r="E35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="60"/>
+      <c r="E36" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="60"/>
+      <c r="E37" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="60"/>
+      <c r="E38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="60"/>
+      <c r="E39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="60"/>
+      <c r="E40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="60"/>
+      <c r="E41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="60"/>
+      <c r="D42" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="60"/>
+      <c r="E43" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="62" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="60"/>
+      <c r="D45" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" s="60"/>
+      <c r="E46" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="60"/>
+      <c r="E47" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" s="60"/>
+      <c r="E48" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="60"/>
+      <c r="E49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="60"/>
+      <c r="D50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="60"/>
+      <c r="E51" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="60"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="62" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" s="57" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="60"/>
+      <c r="D54" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="60"/>
+      <c r="E55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="60"/>
+      <c r="E56" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="60"/>
+      <c r="E57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="60"/>
+      <c r="E58" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="60"/>
+      <c r="E59" t="s">
+        <v>209</v>
+      </c>
+      <c r="H59" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" s="60"/>
+      <c r="E60" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="60"/>
+      <c r="E61" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="2:20">
-      <c r="B24" s="80"/>
-      <c r="E24" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="25" spans="2:20">
-      <c r="B25" s="80"/>
-      <c r="E25" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="2:20">
-      <c r="B26" s="80"/>
-      <c r="E26" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="27" spans="2:20">
-      <c r="B27" s="80"/>
-      <c r="E27" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="28" spans="2:20">
-      <c r="B28" s="80"/>
-      <c r="E28" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="29" spans="2:20">
-      <c r="B29" s="80"/>
-      <c r="E29" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="30" spans="2:20">
-      <c r="B30" s="82" t="s">
+    <row r="62" spans="2:8">
+      <c r="B62" s="60"/>
+      <c r="E62" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="60"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="C30" s="57" t="s">
-        <v>199</v>
-      </c>
-      <c r="H30" s="81" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="31" spans="2:20">
-      <c r="B31" s="80"/>
-      <c r="D31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="32" spans="2:20">
-      <c r="B32" s="80"/>
-      <c r="E32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="80"/>
-      <c r="E33" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="80"/>
-      <c r="E34" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="80"/>
-      <c r="E35" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="80"/>
-      <c r="E36" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="80"/>
-      <c r="E37" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="80"/>
-      <c r="E38" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="80"/>
-      <c r="E39" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="80"/>
-      <c r="E40" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="B41" s="80"/>
-      <c r="E41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="B42" s="80"/>
-      <c r="D42" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="B43" s="80"/>
-      <c r="E43" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="82" t="s">
-        <v>235</v>
-      </c>
-      <c r="C44" s="57" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="B45" s="80"/>
-      <c r="D45" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="B46" s="80"/>
-      <c r="E46" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5">
-      <c r="B47" s="80"/>
-      <c r="E47" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="B48" s="80"/>
-      <c r="E48" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8">
-      <c r="B49" s="80"/>
-      <c r="E49" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" s="80"/>
-      <c r="D50" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" s="80"/>
-      <c r="E51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="80"/>
-    </row>
-    <row r="53" spans="2:8">
-      <c r="B53" s="82" t="s">
-        <v>234</v>
-      </c>
-      <c r="C53" s="57" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8">
-      <c r="B54" s="80"/>
-      <c r="D54" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8">
-      <c r="B55" s="80"/>
-      <c r="E55" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8">
-      <c r="B56" s="80"/>
-      <c r="E56" t="s">
+      <c r="C64" s="57" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="57" spans="2:8">
-      <c r="B57" s="80"/>
-      <c r="E57" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8">
-      <c r="B58" s="80"/>
-      <c r="E58" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8">
-      <c r="B59" s="80"/>
-      <c r="E59" t="s">
-        <v>210</v>
-      </c>
-      <c r="H59" t="s">
+    <row r="65" spans="2:5">
+      <c r="B65" s="59"/>
+      <c r="D65" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="59"/>
+      <c r="E66" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="59"/>
+      <c r="E67" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="59"/>
+      <c r="E68" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="59"/>
+      <c r="E69" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" s="59"/>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="58" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" s="59"/>
+      <c r="C72" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="60" spans="2:8">
-      <c r="B60" s="80"/>
-      <c r="E60" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8">
-      <c r="B61" s="80"/>
-      <c r="E61" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8">
-      <c r="B62" s="80"/>
-      <c r="E62" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" s="80"/>
-    </row>
-    <row r="64" spans="2:8">
-      <c r="B64" s="82" t="s">
-        <v>235</v>
-      </c>
-      <c r="C64" s="57" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5">
-      <c r="B65" s="79"/>
-      <c r="D65" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5">
-      <c r="B66" s="79"/>
-      <c r="E66" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5">
-      <c r="B67" s="79"/>
-      <c r="E67" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5">
-      <c r="B68" s="79"/>
-      <c r="E68" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5">
-      <c r="B69" s="79"/>
-      <c r="E69" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5">
-      <c r="B70" s="79"/>
-    </row>
-    <row r="71" spans="2:5">
-      <c r="B71" s="78" t="s">
+    <row r="73" spans="2:5">
+      <c r="B73" s="59"/>
+      <c r="C73" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="B74" s="59"/>
+      <c r="C74" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75" s="59"/>
+    </row>
+    <row r="76" spans="2:5">
+      <c r="B76" s="58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="72" spans="2:5">
-      <c r="B72" s="79"/>
-      <c r="C72" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5">
-      <c r="B73" s="79"/>
-      <c r="C73" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5">
-      <c r="B74" s="79"/>
-      <c r="C74" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5">
-      <c r="B75" s="79"/>
-    </row>
-    <row r="76" spans="2:5">
-      <c r="B76" s="78" t="s">
-        <v>187</v>
-      </c>
-    </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="79"/>
+      <c r="B81" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5666,15 +5666,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="57" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B1" t="s">
         <v>143</v>
@@ -5684,147 +5684,147 @@
       <c r="B2" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
     </row>
     <row r="3" spans="1:16">
       <c r="B3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="F4" s="61" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="F4" s="81" t="s">
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="F5" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="F5" s="81" t="s">
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="F6" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="F6" s="81" t="s">
-        <v>183</v>
-      </c>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="81"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
     </row>
     <row r="7" spans="1:16">
       <c r="B7" t="s">
+        <v>235</v>
+      </c>
+      <c r="F7" s="61" t="s">
         <v>236</v>
       </c>
-      <c r="F7" s="81" t="s">
-        <v>237</v>
-      </c>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
     </row>
     <row r="8" spans="1:16">
       <c r="B8" t="s">
-        <v>240</v>
-      </c>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="81"/>
+        <v>239</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
     </row>
     <row r="9" spans="1:16">
       <c r="B9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F9" s="61" t="s">
         <v>241</v>
       </c>
-      <c r="F9" s="81" t="s">
-        <v>242</v>
-      </c>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
     </row>
     <row r="15" spans="1:16">
       <c r="B15" t="s">
@@ -5879,13 +5879,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -5893,66 +5893,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="67" t="s">
+      <c r="K2" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="69"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="67"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="67" t="s">
+      <c r="Q2" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="69"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="67"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="59" t="s">
+      <c r="V2" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="61"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="76"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="62" t="s">
+      <c r="AA2" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="64"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="79"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="59" t="s">
+      <c r="AI2" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="60"/>
-      <c r="AP2" s="60"/>
+      <c r="AJ2" s="75"/>
+      <c r="AK2" s="75"/>
+      <c r="AL2" s="75"/>
+      <c r="AM2" s="75"/>
+      <c r="AN2" s="75"/>
+      <c r="AO2" s="75"/>
+      <c r="AP2" s="75"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="G3" s="80" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -5979,12 +5979,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="73"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Done Bs-Pagination Component (Shared Module)
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -1253,7 +1253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1298,6 +1298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1541,7 +1547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1749,6 +1755,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="% complete" xfId="12"/>
@@ -2340,7 +2350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -2529,7 +2539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -2857,7 +2867,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:O2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="30" customHeight="1"/>
@@ -3343,7 +3353,7 @@
         <v>94</v>
       </c>
       <c r="H7"/>
-      <c r="I7" s="17"/>
+      <c r="I7" s="16"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -3409,7 +3419,7 @@
       </c>
       <c r="H8"/>
       <c r="I8"/>
-      <c r="J8" s="18"/>
+      <c r="J8" s="17"/>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
@@ -4949,9 +4959,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2 H5 I6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 I7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2 N11:V11 X13:X14 J8:M8 M10:U10 W12:X12 W13 M9:N9"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2 H5 I6:I7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 J8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2 N11:V11 X13:X14 M9:N9 M10:U10 W12:X12 W13 K8:M8"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
@@ -5071,10 +5081,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T81"/>
+  <dimension ref="A2:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5095,7 +5105,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" ht="15.75" thickBot="1">
       <c r="B4" s="57" t="s">
         <v>184</v>
       </c>
@@ -5104,9 +5114,12 @@
       <c r="B5" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="83" t="s">
         <v>195</v>
       </c>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
       <c r="H5" s="61" t="s">
         <v>228</v>
       </c>
@@ -5116,25 +5129,34 @@
     </row>
     <row r="6" spans="1:20">
       <c r="B6" s="60"/>
-      <c r="D6" t="s">
+      <c r="C6" s="51"/>
+      <c r="D6" s="86" t="s">
         <v>187</v>
       </c>
+      <c r="E6" s="52"/>
+      <c r="F6" s="53"/>
       <c r="M6" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1">
       <c r="B7" s="60"/>
-      <c r="E7" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52" t="s">
         <v>154</v>
       </c>
+      <c r="F7" s="53"/>
       <c r="S7" s="52"/>
     </row>
     <row r="8" spans="1:20">
       <c r="B8" s="60"/>
-      <c r="E8" t="s">
+      <c r="C8" s="51"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="84" t="s">
         <v>208</v>
       </c>
+      <c r="F8" s="85"/>
       <c r="N8" s="48" t="s">
         <v>150</v>
       </c>
@@ -5147,9 +5169,12 @@
     </row>
     <row r="9" spans="1:20">
       <c r="B9" s="60"/>
-      <c r="E9" t="s">
+      <c r="C9" s="51"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52" t="s">
         <v>237</v>
       </c>
+      <c r="F9" s="53"/>
       <c r="N9" s="51"/>
       <c r="O9" s="52" t="s">
         <v>170</v>
@@ -5162,9 +5187,12 @@
     </row>
     <row r="10" spans="1:20">
       <c r="B10" s="60"/>
-      <c r="D10" t="s">
+      <c r="C10" s="51"/>
+      <c r="D10" s="86" t="s">
         <v>188</v>
       </c>
+      <c r="E10" s="52"/>
+      <c r="F10" s="53"/>
       <c r="N10" s="51"/>
       <c r="O10" s="52" t="s">
         <v>151</v>
@@ -5179,9 +5207,12 @@
     </row>
     <row r="11" spans="1:20">
       <c r="B11" s="60"/>
-      <c r="E11" t="s">
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52" t="s">
         <v>189</v>
       </c>
+      <c r="F11" s="53"/>
       <c r="N11" s="51"/>
       <c r="O11" s="52" t="s">
         <v>165</v>
@@ -5194,9 +5225,12 @@
     </row>
     <row r="12" spans="1:20">
       <c r="B12" s="60"/>
-      <c r="E12" t="s">
+      <c r="C12" s="51"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52" t="s">
         <v>190</v>
       </c>
+      <c r="F12" s="53"/>
       <c r="N12" s="51" t="s">
         <v>156</v>
       </c>
@@ -5209,9 +5243,12 @@
     </row>
     <row r="13" spans="1:20">
       <c r="B13" s="60"/>
-      <c r="E13" t="s">
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52" t="s">
         <v>194</v>
       </c>
+      <c r="F13" s="53"/>
       <c r="N13" s="51" t="s">
         <v>174</v>
       </c>
@@ -5224,9 +5261,12 @@
     </row>
     <row r="14" spans="1:20">
       <c r="B14" s="60"/>
-      <c r="E14" t="s">
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52" t="s">
         <v>191</v>
       </c>
+      <c r="F14" s="53"/>
       <c r="N14" s="51"/>
       <c r="O14" s="52" t="s">
         <v>175</v>
@@ -5239,9 +5279,12 @@
     </row>
     <row r="15" spans="1:20">
       <c r="B15" s="60"/>
-      <c r="D15" t="s">
+      <c r="C15" s="51"/>
+      <c r="D15" s="86" t="s">
         <v>177</v>
       </c>
+      <c r="E15" s="52"/>
+      <c r="F15" s="53"/>
       <c r="N15" s="51"/>
       <c r="O15" s="52"/>
       <c r="P15" s="52" t="s">
@@ -5254,9 +5297,12 @@
     </row>
     <row r="16" spans="1:20">
       <c r="B16" s="60"/>
-      <c r="E16" t="s">
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52" t="s">
         <v>192</v>
       </c>
+      <c r="F16" s="53"/>
       <c r="N16" s="51"/>
       <c r="O16" s="52"/>
       <c r="P16" s="52"/>
@@ -5271,9 +5317,12 @@
     </row>
     <row r="17" spans="2:20">
       <c r="B17" s="60"/>
-      <c r="E17" t="s">
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52" t="s">
         <v>193</v>
       </c>
+      <c r="F17" s="53"/>
       <c r="N17" s="51"/>
       <c r="O17" s="52"/>
       <c r="P17" s="52" t="s">
@@ -5286,9 +5335,12 @@
     </row>
     <row r="18" spans="2:20" ht="15.75" thickBot="1">
       <c r="B18" s="60"/>
-      <c r="E18" t="s">
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52" t="s">
         <v>168</v>
       </c>
+      <c r="F18" s="53"/>
       <c r="N18" s="54" t="s">
         <v>157</v>
       </c>
@@ -5299,19 +5351,25 @@
       <c r="S18" s="55"/>
       <c r="T18" s="56"/>
     </row>
-    <row r="19" spans="2:20">
+    <row r="19" spans="2:20" ht="15.75" thickBot="1">
       <c r="B19" s="60"/>
-      <c r="E19" t="s">
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55" t="s">
         <v>155</v>
       </c>
+      <c r="F19" s="56"/>
     </row>
     <row r="20" spans="2:20">
       <c r="B20" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="83" t="s">
         <v>199</v>
       </c>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
       <c r="H20" s="61" t="s">
         <v>229</v>
       </c>
@@ -5319,342 +5377,487 @@
     </row>
     <row r="21" spans="2:20">
       <c r="B21" s="60"/>
-      <c r="D21" t="s">
+      <c r="C21" s="51"/>
+      <c r="D21" s="86" t="s">
         <v>196</v>
       </c>
+      <c r="E21" s="52"/>
+      <c r="F21" s="53"/>
     </row>
     <row r="22" spans="2:20">
       <c r="B22" s="60"/>
-      <c r="E22" t="s">
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52" t="s">
         <v>150</v>
       </c>
+      <c r="F22" s="53"/>
     </row>
     <row r="23" spans="2:20">
       <c r="B23" s="60"/>
-      <c r="E23" t="s">
+      <c r="C23" s="51"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52" t="s">
         <v>157</v>
       </c>
+      <c r="F23" s="53"/>
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="60"/>
-      <c r="E24" t="s">
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52" t="s">
         <v>238</v>
       </c>
+      <c r="F24" s="53"/>
     </row>
     <row r="25" spans="2:20">
       <c r="B25" s="60"/>
-      <c r="E25" t="s">
+      <c r="C25" s="51"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52" t="s">
         <v>197</v>
       </c>
+      <c r="F25" s="53"/>
     </row>
     <row r="26" spans="2:20">
       <c r="B26" s="60"/>
-      <c r="E26" t="s">
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52" t="s">
         <v>204</v>
       </c>
+      <c r="F26" s="53"/>
     </row>
     <row r="27" spans="2:20">
       <c r="B27" s="60"/>
-      <c r="E27" t="s">
+      <c r="C27" s="51"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52" t="s">
         <v>205</v>
       </c>
+      <c r="F27" s="53"/>
     </row>
     <row r="28" spans="2:20">
       <c r="B28" s="60"/>
-      <c r="E28" t="s">
+      <c r="C28" s="51"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="29" spans="2:20">
+      <c r="F28" s="53"/>
+    </row>
+    <row r="29" spans="2:20" ht="15.75" thickBot="1">
       <c r="B29" s="60"/>
-      <c r="E29" t="s">
+      <c r="C29" s="54"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55" t="s">
         <v>207</v>
       </c>
+      <c r="F29" s="56"/>
     </row>
     <row r="30" spans="2:20">
       <c r="B30" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="83" t="s">
         <v>198</v>
       </c>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="50"/>
       <c r="H30" s="61" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="31" spans="2:20">
       <c r="B31" s="60"/>
-      <c r="D31" t="s">
+      <c r="C31" s="51"/>
+      <c r="D31" s="86" t="s">
         <v>196</v>
       </c>
+      <c r="E31" s="52"/>
+      <c r="F31" s="53"/>
     </row>
     <row r="32" spans="2:20">
       <c r="B32" s="60"/>
-      <c r="E32" t="s">
+      <c r="C32" s="51"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="33" spans="2:5">
+      <c r="F32" s="53"/>
+    </row>
+    <row r="33" spans="2:6">
       <c r="B33" s="60"/>
-      <c r="E33" t="s">
+      <c r="C33" s="51"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="34" spans="2:5">
+      <c r="F33" s="53"/>
+    </row>
+    <row r="34" spans="2:6">
       <c r="B34" s="60"/>
-      <c r="E34" t="s">
+      <c r="C34" s="51"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="35" spans="2:5">
+      <c r="F34" s="53"/>
+    </row>
+    <row r="35" spans="2:6">
       <c r="B35" s="60"/>
-      <c r="E35" t="s">
+      <c r="C35" s="51"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="36" spans="2:5">
+      <c r="F35" s="53"/>
+    </row>
+    <row r="36" spans="2:6">
       <c r="B36" s="60"/>
-      <c r="E36" t="s">
+      <c r="C36" s="51"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="37" spans="2:5">
+      <c r="F36" s="53"/>
+    </row>
+    <row r="37" spans="2:6">
       <c r="B37" s="60"/>
-      <c r="E37" t="s">
+      <c r="C37" s="51"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="38" spans="2:5">
+      <c r="F37" s="53"/>
+    </row>
+    <row r="38" spans="2:6">
       <c r="B38" s="60"/>
-      <c r="E38" t="s">
+      <c r="C38" s="51"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="39" spans="2:5">
+      <c r="F38" s="53"/>
+    </row>
+    <row r="39" spans="2:6">
       <c r="B39" s="60"/>
-      <c r="E39" t="s">
+      <c r="C39" s="51"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="40" spans="2:5">
+      <c r="F39" s="53"/>
+    </row>
+    <row r="40" spans="2:6">
       <c r="B40" s="60"/>
-      <c r="E40" t="s">
+      <c r="C40" s="51"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="41" spans="2:5">
+      <c r="F40" s="53"/>
+    </row>
+    <row r="41" spans="2:6">
       <c r="B41" s="60"/>
-      <c r="E41" t="s">
+      <c r="C41" s="51"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="42" spans="2:5">
+      <c r="F41" s="53"/>
+    </row>
+    <row r="42" spans="2:6">
       <c r="B42" s="60"/>
-      <c r="D42" t="s">
+      <c r="C42" s="51"/>
+      <c r="D42" s="86" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="43" spans="2:5">
+      <c r="E42" s="52"/>
+      <c r="F42" s="53"/>
+    </row>
+    <row r="43" spans="2:6" ht="15.75" thickBot="1">
       <c r="B43" s="60"/>
-      <c r="E43" t="s">
+      <c r="C43" s="54"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="44" spans="2:5">
+      <c r="F43" s="56"/>
+    </row>
+    <row r="44" spans="2:6">
       <c r="B44" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="83" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="45" spans="2:5">
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="50"/>
+    </row>
+    <row r="45" spans="2:6">
       <c r="B45" s="60"/>
-      <c r="D45" t="s">
+      <c r="C45" s="51"/>
+      <c r="D45" s="86" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="46" spans="2:5">
+      <c r="E45" s="52"/>
+      <c r="F45" s="53"/>
+    </row>
+    <row r="46" spans="2:6">
       <c r="B46" s="60"/>
-      <c r="E46" t="s">
+      <c r="C46" s="51"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="47" spans="2:5">
+      <c r="F46" s="53"/>
+    </row>
+    <row r="47" spans="2:6">
       <c r="B47" s="60"/>
-      <c r="E47" t="s">
+      <c r="C47" s="51"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="48" spans="2:5">
+      <c r="F47" s="53"/>
+    </row>
+    <row r="48" spans="2:6">
       <c r="B48" s="60"/>
-      <c r="E48" t="s">
+      <c r="C48" s="51"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52" t="s">
         <v>220</v>
       </c>
+      <c r="F48" s="53"/>
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="60"/>
-      <c r="E49" t="s">
+      <c r="C49" s="51"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52" t="s">
         <v>162</v>
       </c>
+      <c r="F49" s="53"/>
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="60"/>
-      <c r="D50" t="s">
+      <c r="C50" s="51"/>
+      <c r="D50" s="86" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="51" spans="2:8">
+      <c r="E50" s="52"/>
+      <c r="F50" s="53"/>
+    </row>
+    <row r="51" spans="2:8" ht="15.75" thickBot="1">
       <c r="B51" s="60"/>
-      <c r="E51" t="s">
+      <c r="C51" s="54"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55" t="s">
         <v>215</v>
       </c>
+      <c r="F51" s="56"/>
     </row>
     <row r="52" spans="2:8">
-      <c r="B52" s="60"/>
+      <c r="B52" s="62" t="s">
+        <v>233</v>
+      </c>
+      <c r="C52" s="83" t="s">
+        <v>222</v>
+      </c>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="50"/>
     </row>
     <row r="53" spans="2:8">
-      <c r="B53" s="62" t="s">
-        <v>233</v>
-      </c>
-      <c r="C53" s="57" t="s">
-        <v>222</v>
-      </c>
+      <c r="B53" s="60"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="86" t="s">
+        <v>196</v>
+      </c>
+      <c r="E53" s="52"/>
+      <c r="F53" s="53"/>
     </row>
     <row r="54" spans="2:8">
       <c r="B54" s="60"/>
-      <c r="D54" t="s">
-        <v>196</v>
-      </c>
+      <c r="C54" s="51"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="F54" s="53"/>
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="60"/>
-      <c r="E55" t="s">
-        <v>169</v>
-      </c>
+      <c r="C55" s="51"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="F55" s="53"/>
     </row>
     <row r="56" spans="2:8">
       <c r="B56" s="60"/>
-      <c r="E56" t="s">
-        <v>223</v>
-      </c>
+      <c r="C56" s="51"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="F56" s="53"/>
     </row>
     <row r="57" spans="2:8">
       <c r="B57" s="60"/>
-      <c r="E57" t="s">
-        <v>171</v>
-      </c>
+      <c r="C57" s="51"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="F57" s="53"/>
     </row>
     <row r="58" spans="2:8">
       <c r="B58" s="60"/>
-      <c r="E58" t="s">
-        <v>167</v>
+      <c r="C58" s="51"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="F58" s="53"/>
+      <c r="H58" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="2:8">
       <c r="B59" s="60"/>
-      <c r="E59" t="s">
-        <v>209</v>
-      </c>
-      <c r="H59" t="s">
-        <v>210</v>
-      </c>
+      <c r="C59" s="51"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="F59" s="53"/>
     </row>
     <row r="60" spans="2:8">
       <c r="B60" s="60"/>
-      <c r="E60" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8">
+      <c r="C60" s="51"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="F60" s="53"/>
+    </row>
+    <row r="61" spans="2:8" ht="15.75" thickBot="1">
       <c r="B61" s="60"/>
-      <c r="E61" t="s">
-        <v>158</v>
-      </c>
+      <c r="C61" s="54"/>
+      <c r="D61" s="55"/>
+      <c r="E61" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="F61" s="56"/>
     </row>
     <row r="62" spans="2:8">
-      <c r="B62" s="60"/>
-      <c r="E62" t="s">
-        <v>159</v>
-      </c>
+      <c r="B62" s="62" t="s">
+        <v>234</v>
+      </c>
+      <c r="C62" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="D62" s="49"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="50"/>
     </row>
     <row r="63" spans="2:8">
-      <c r="B63" s="60"/>
+      <c r="B63" s="59"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="86" t="s">
+        <v>196</v>
+      </c>
+      <c r="E63" s="52"/>
+      <c r="F63" s="53"/>
     </row>
     <row r="64" spans="2:8">
-      <c r="B64" s="62" t="s">
-        <v>234</v>
-      </c>
-      <c r="C64" s="57" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5">
+      <c r="B64" s="59"/>
+      <c r="C64" s="51"/>
+      <c r="D64" s="52"/>
+      <c r="E64" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="F64" s="53"/>
+    </row>
+    <row r="65" spans="2:6">
       <c r="B65" s="59"/>
-      <c r="D65" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5">
+      <c r="C65" s="51"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="52" t="s">
+        <v>225</v>
+      </c>
+      <c r="F65" s="53"/>
+    </row>
+    <row r="66" spans="2:6">
       <c r="B66" s="59"/>
-      <c r="E66" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5">
+      <c r="C66" s="51"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="F66" s="53"/>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" thickBot="1">
       <c r="B67" s="59"/>
-      <c r="E67" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5">
-      <c r="B68" s="59"/>
-      <c r="E68" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5">
+      <c r="C67" s="54"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="F67" s="56"/>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B68" s="58" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
       <c r="B69" s="59"/>
-      <c r="E69" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5">
+      <c r="C69" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="D69" s="49"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="50"/>
+    </row>
+    <row r="70" spans="2:6">
       <c r="B70" s="59"/>
-    </row>
-    <row r="71" spans="2:5">
-      <c r="B71" s="58" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5">
+      <c r="C70" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
+      <c r="F70" s="53"/>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="59"/>
+      <c r="C71" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="D71" s="52"/>
+      <c r="E71" s="52"/>
+      <c r="F71" s="53"/>
+    </row>
+    <row r="72" spans="2:6" ht="15.75" thickBot="1">
       <c r="B72" s="59"/>
-      <c r="C72" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5">
-      <c r="B73" s="59"/>
-      <c r="C73" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5">
-      <c r="B74" s="59"/>
-      <c r="C74" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5">
-      <c r="B75" s="59"/>
-    </row>
-    <row r="76" spans="2:5">
-      <c r="B76" s="58" t="s">
+      <c r="C72" s="54"/>
+      <c r="D72" s="55"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="56"/>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="2:2">
-      <c r="B81" s="59"/>
+    <row r="78" spans="2:6">
+      <c r="B78" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Done Bs-Rating Component (Shared Module)
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -901,9 +901,6 @@
     <t>bs-breadcrumb</t>
   </si>
   <si>
-    <t>rating</t>
-  </si>
-  <si>
     <t>(kèm sao và số lượt đánh giá)</t>
   </si>
   <si>
@@ -1001,6 +998,9 @@
   </si>
   <si>
     <t>Components (outdated)</t>
+  </si>
+  <si>
+    <t>bs-rating</t>
   </si>
 </sst>
 </file>
@@ -1547,7 +1547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1695,70 +1695,71 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="% complete" xfId="12"/>
@@ -2888,41 +2889,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73" t="s">
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
-      <c r="AB1" s="73"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -2930,66 +2931,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="65" t="s">
+      <c r="K2" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="65" t="s">
+      <c r="Q2" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="67"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="71"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="74" t="s">
+      <c r="V2" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="76"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="80"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="77" t="s">
+      <c r="AA2" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="79"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="82"/>
+      <c r="AF2" s="82"/>
+      <c r="AG2" s="83"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="74" t="s">
+      <c r="AI2" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="75"/>
-      <c r="AP2" s="75"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="79"/>
+      <c r="AN2" s="79"/>
+      <c r="AO2" s="79"/>
+      <c r="AP2" s="79"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="67" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -3016,12 +3017,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="71"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>
@@ -5083,8 +5084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5096,7 +5097,7 @@
   <sheetData>
     <row r="2" spans="1:20">
       <c r="A2" s="57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N2" s="57"/>
     </row>
@@ -5112,25 +5113,25 @@
     </row>
     <row r="5" spans="1:20">
       <c r="B5" s="62" t="s">
-        <v>233</v>
-      </c>
-      <c r="C5" s="83" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="63" t="s">
         <v>195</v>
       </c>
       <c r="D5" s="49"/>
       <c r="E5" s="49"/>
       <c r="F5" s="50"/>
       <c r="H5" s="61" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M5" s="57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="B6" s="60"/>
       <c r="C6" s="51"/>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="66" t="s">
         <v>187</v>
       </c>
       <c r="E6" s="52"/>
@@ -5153,10 +5154,10 @@
       <c r="B8" s="60"/>
       <c r="C8" s="51"/>
       <c r="D8" s="52"/>
-      <c r="E8" s="84" t="s">
+      <c r="E8" s="64" t="s">
         <v>208</v>
       </c>
-      <c r="F8" s="85"/>
+      <c r="F8" s="65"/>
       <c r="N8" s="48" t="s">
         <v>150</v>
       </c>
@@ -5171,10 +5172,10 @@
       <c r="B9" s="60"/>
       <c r="C9" s="51"/>
       <c r="D9" s="52"/>
-      <c r="E9" s="52" t="s">
-        <v>237</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="64" t="s">
+        <v>236</v>
+      </c>
+      <c r="F9" s="65"/>
       <c r="N9" s="51"/>
       <c r="O9" s="52" t="s">
         <v>170</v>
@@ -5188,19 +5189,18 @@
     <row r="10" spans="1:20">
       <c r="B10" s="60"/>
       <c r="C10" s="51"/>
-      <c r="D10" s="86" t="s">
-        <v>188</v>
-      </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" s="87"/>
+      <c r="H10" t="s">
+        <v>209</v>
+      </c>
       <c r="N10" s="51"/>
-      <c r="O10" s="52" t="s">
-        <v>151</v>
-      </c>
+      <c r="O10" s="52"/>
       <c r="P10" s="52"/>
-      <c r="Q10" s="52" t="s">
-        <v>173</v>
-      </c>
+      <c r="Q10" s="52"/>
       <c r="R10" s="52"/>
       <c r="S10" s="52"/>
       <c r="T10" s="53"/>
@@ -5208,17 +5208,19 @@
     <row r="11" spans="1:20">
       <c r="B11" s="60"/>
       <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52" t="s">
-        <v>189</v>
-      </c>
+      <c r="D11" s="66" t="s">
+        <v>188</v>
+      </c>
+      <c r="E11" s="52"/>
       <c r="F11" s="53"/>
       <c r="N11" s="51"/>
       <c r="O11" s="52" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="P11" s="52"/>
-      <c r="Q11" s="52"/>
+      <c r="Q11" s="52" t="s">
+        <v>173</v>
+      </c>
       <c r="R11" s="52"/>
       <c r="S11" s="52"/>
       <c r="T11" s="53"/>
@@ -5228,13 +5230,13 @@
       <c r="C12" s="51"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F12" s="53"/>
-      <c r="N12" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="O12" s="52"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="52" t="s">
+        <v>165</v>
+      </c>
       <c r="P12" s="52"/>
       <c r="Q12" s="52"/>
       <c r="R12" s="52"/>
@@ -5246,11 +5248,11 @@
       <c r="C13" s="51"/>
       <c r="D13" s="52"/>
       <c r="E13" s="52" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F13" s="53"/>
       <c r="N13" s="51" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="O13" s="52"/>
       <c r="P13" s="52"/>
@@ -5264,13 +5266,13 @@
       <c r="C14" s="51"/>
       <c r="D14" s="52"/>
       <c r="E14" s="52" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F14" s="53"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="52" t="s">
-        <v>175</v>
-      </c>
+      <c r="N14" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="O14" s="52"/>
       <c r="P14" s="52"/>
       <c r="Q14" s="52"/>
       <c r="R14" s="52"/>
@@ -5280,16 +5282,16 @@
     <row r="15" spans="1:20">
       <c r="B15" s="60"/>
       <c r="C15" s="51"/>
-      <c r="D15" s="86" t="s">
-        <v>177</v>
-      </c>
-      <c r="E15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52" t="s">
+        <v>191</v>
+      </c>
       <c r="F15" s="53"/>
       <c r="N15" s="51"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="52" t="s">
-        <v>176</v>
-      </c>
+      <c r="O15" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="P15" s="52"/>
       <c r="Q15" s="52"/>
       <c r="R15" s="52"/>
       <c r="S15" s="52"/>
@@ -5298,21 +5300,19 @@
     <row r="16" spans="1:20">
       <c r="B16" s="60"/>
       <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52" t="s">
-        <v>192</v>
-      </c>
+      <c r="D16" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="52"/>
       <c r="F16" s="53"/>
       <c r="N16" s="51"/>
       <c r="O16" s="52"/>
-      <c r="P16" s="52"/>
+      <c r="P16" s="52" t="s">
+        <v>176</v>
+      </c>
       <c r="Q16" s="52"/>
-      <c r="R16" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="S16" s="52" t="s">
-        <v>172</v>
-      </c>
+      <c r="R16" s="52"/>
+      <c r="S16" s="52"/>
       <c r="T16" s="53"/>
     </row>
     <row r="17" spans="2:20">
@@ -5320,77 +5320,88 @@
       <c r="C17" s="51"/>
       <c r="D17" s="52"/>
       <c r="E17" s="52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F17" s="53"/>
       <c r="N17" s="51"/>
       <c r="O17" s="52"/>
-      <c r="P17" s="52" t="s">
-        <v>163</v>
-      </c>
+      <c r="P17" s="52"/>
       <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="52"/>
+      <c r="R17" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="S17" s="52" t="s">
+        <v>172</v>
+      </c>
       <c r="T17" s="53"/>
     </row>
-    <row r="18" spans="2:20" ht="15.75" thickBot="1">
+    <row r="18" spans="2:20">
       <c r="B18" s="60"/>
       <c r="C18" s="51"/>
       <c r="D18" s="52"/>
       <c r="E18" s="52" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="F18" s="53"/>
-      <c r="N18" s="54" t="s">
-        <v>157</v>
-      </c>
-      <c r="O18" s="55"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="55"/>
-      <c r="S18" s="55"/>
-      <c r="T18" s="56"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="52"/>
+      <c r="T18" s="53"/>
     </row>
     <row r="19" spans="2:20" ht="15.75" thickBot="1">
       <c r="B19" s="60"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55" t="s">
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" s="53"/>
+      <c r="N19" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="56"/>
+    </row>
+    <row r="20" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B20" s="60"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="F19" s="56"/>
-    </row>
-    <row r="20" spans="2:20">
-      <c r="B20" s="62" t="s">
-        <v>234</v>
-      </c>
-      <c r="C20" s="83" t="s">
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="2:20">
+      <c r="B21" s="62" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21" s="63" t="s">
         <v>199</v>
       </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="50"/>
-      <c r="H20" s="61" t="s">
-        <v>229</v>
-      </c>
-      <c r="S20" s="52"/>
-    </row>
-    <row r="21" spans="2:20">
-      <c r="B21" s="60"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="86" t="s">
-        <v>196</v>
-      </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="53"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="H21" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="S21" s="52"/>
     </row>
     <row r="22" spans="2:20">
       <c r="B22" s="60"/>
       <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52" t="s">
-        <v>150</v>
-      </c>
+      <c r="D22" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E22" s="52"/>
       <c r="F22" s="53"/>
     </row>
     <row r="23" spans="2:20">
@@ -5398,7 +5409,7 @@
       <c r="C23" s="51"/>
       <c r="D23" s="52"/>
       <c r="E23" s="52" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F23" s="53"/>
     </row>
@@ -5407,7 +5418,7 @@
       <c r="C24" s="51"/>
       <c r="D24" s="52"/>
       <c r="E24" s="52" t="s">
-        <v>238</v>
+        <v>157</v>
       </c>
       <c r="F24" s="53"/>
     </row>
@@ -5416,7 +5427,7 @@
       <c r="C25" s="51"/>
       <c r="D25" s="52"/>
       <c r="E25" s="52" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="F25" s="53"/>
     </row>
@@ -5425,7 +5436,7 @@
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="52" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F26" s="53"/>
     </row>
@@ -5434,7 +5445,7 @@
       <c r="C27" s="51"/>
       <c r="D27" s="52"/>
       <c r="E27" s="52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F27" s="53"/>
     </row>
@@ -5443,49 +5454,49 @@
       <c r="C28" s="51"/>
       <c r="D28" s="52"/>
       <c r="E28" s="52" t="s">
+        <v>205</v>
+      </c>
+      <c r="F28" s="53"/>
+    </row>
+    <row r="29" spans="2:20">
+      <c r="B29" s="60"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="F28" s="53"/>
-    </row>
-    <row r="29" spans="2:20" ht="15.75" thickBot="1">
-      <c r="B29" s="60"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55" t="s">
+      <c r="F29" s="53"/>
+    </row>
+    <row r="30" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B30" s="60"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="F29" s="56"/>
-    </row>
-    <row r="30" spans="2:20">
-      <c r="B30" s="62" t="s">
-        <v>233</v>
-      </c>
-      <c r="C30" s="83" t="s">
+      <c r="F30" s="56"/>
+    </row>
+    <row r="31" spans="2:20">
+      <c r="B31" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" s="63" t="s">
         <v>198</v>
       </c>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="50"/>
-      <c r="H30" s="61" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="31" spans="2:20">
-      <c r="B31" s="60"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="86" t="s">
-        <v>196</v>
-      </c>
-      <c r="E31" s="52"/>
-      <c r="F31" s="53"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50"/>
+      <c r="H31" s="61" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="32" spans="2:20">
       <c r="B32" s="60"/>
       <c r="C32" s="51"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52" t="s">
-        <v>151</v>
-      </c>
+      <c r="D32" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32" s="52"/>
       <c r="F32" s="53"/>
     </row>
     <row r="33" spans="2:6">
@@ -5493,7 +5504,7 @@
       <c r="C33" s="51"/>
       <c r="D33" s="52"/>
       <c r="E33" s="52" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="F33" s="53"/>
     </row>
@@ -5502,7 +5513,7 @@
       <c r="C34" s="51"/>
       <c r="D34" s="52"/>
       <c r="E34" s="52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F34" s="53"/>
     </row>
@@ -5511,7 +5522,7 @@
       <c r="C35" s="51"/>
       <c r="D35" s="52"/>
       <c r="E35" s="52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F35" s="53"/>
     </row>
@@ -5520,7 +5531,7 @@
       <c r="C36" s="51"/>
       <c r="D36" s="52"/>
       <c r="E36" s="52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F36" s="53"/>
     </row>
@@ -5529,7 +5540,7 @@
       <c r="C37" s="51"/>
       <c r="D37" s="52"/>
       <c r="E37" s="52" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="F37" s="53"/>
     </row>
@@ -5538,7 +5549,7 @@
       <c r="C38" s="51"/>
       <c r="D38" s="52"/>
       <c r="E38" s="52" t="s">
-        <v>160</v>
+        <v>215</v>
       </c>
       <c r="F38" s="53"/>
     </row>
@@ -5547,7 +5558,7 @@
       <c r="C39" s="51"/>
       <c r="D39" s="52"/>
       <c r="E39" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F39" s="53"/>
     </row>
@@ -5556,7 +5567,7 @@
       <c r="C40" s="51"/>
       <c r="D40" s="52"/>
       <c r="E40" s="52" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F40" s="53"/>
     </row>
@@ -5565,55 +5576,55 @@
       <c r="C41" s="51"/>
       <c r="D41" s="52"/>
       <c r="E41" s="52" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F41" s="53"/>
     </row>
     <row r="42" spans="2:6">
       <c r="B42" s="60"/>
       <c r="C42" s="51"/>
-      <c r="D42" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="E42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52" t="s">
+        <v>152</v>
+      </c>
       <c r="F42" s="53"/>
     </row>
-    <row r="43" spans="2:6" ht="15.75" thickBot="1">
+    <row r="43" spans="2:6">
       <c r="B43" s="60"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55" t="s">
-        <v>221</v>
-      </c>
-      <c r="F43" s="56"/>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="B44" s="62" t="s">
-        <v>234</v>
-      </c>
-      <c r="C44" s="83" t="s">
-        <v>214</v>
-      </c>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="50"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="66" t="s">
+        <v>216</v>
+      </c>
+      <c r="E43" s="52"/>
+      <c r="F43" s="53"/>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B44" s="60"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="F44" s="56"/>
     </row>
     <row r="45" spans="2:6">
-      <c r="B45" s="60"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="86" t="s">
-        <v>196</v>
-      </c>
-      <c r="E45" s="52"/>
-      <c r="F45" s="53"/>
+      <c r="B45" s="62" t="s">
+        <v>233</v>
+      </c>
+      <c r="C45" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="50"/>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" s="60"/>
       <c r="C46" s="51"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52" t="s">
-        <v>218</v>
-      </c>
+      <c r="D46" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E46" s="52"/>
       <c r="F46" s="53"/>
     </row>
     <row r="47" spans="2:6">
@@ -5621,7 +5632,7 @@
       <c r="C47" s="51"/>
       <c r="D47" s="52"/>
       <c r="E47" s="52" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F47" s="53"/>
     </row>
@@ -5630,106 +5641,103 @@
       <c r="C48" s="51"/>
       <c r="D48" s="52"/>
       <c r="E48" s="52" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F48" s="53"/>
     </row>
-    <row r="49" spans="2:8">
+    <row r="49" spans="2:6">
       <c r="B49" s="60"/>
       <c r="C49" s="51"/>
       <c r="D49" s="52"/>
       <c r="E49" s="52" t="s">
-        <v>162</v>
+        <v>219</v>
       </c>
       <c r="F49" s="53"/>
     </row>
-    <row r="50" spans="2:8">
+    <row r="50" spans="2:6">
       <c r="B50" s="60"/>
       <c r="C50" s="51"/>
-      <c r="D50" s="86" t="s">
+      <c r="D50" s="52"/>
+      <c r="E50" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="F50" s="53"/>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="60"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="E50" s="52"/>
-      <c r="F50" s="53"/>
-    </row>
-    <row r="51" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B51" s="60"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55" t="s">
-        <v>215</v>
-      </c>
-      <c r="F51" s="56"/>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="62" t="s">
-        <v>233</v>
-      </c>
-      <c r="C52" s="83" t="s">
-        <v>222</v>
-      </c>
-      <c r="D52" s="49"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="50"/>
-    </row>
-    <row r="53" spans="2:8">
-      <c r="B53" s="60"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="86" t="s">
-        <v>196</v>
-      </c>
-      <c r="E53" s="52"/>
-      <c r="F53" s="53"/>
-    </row>
-    <row r="54" spans="2:8">
+      <c r="E51" s="52"/>
+      <c r="F51" s="53"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B52" s="60"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="F52" s="56"/>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" s="63" t="s">
+        <v>221</v>
+      </c>
+      <c r="D53" s="49"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="50"/>
+    </row>
+    <row r="54" spans="2:6">
       <c r="B54" s="60"/>
       <c r="C54" s="51"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="52" t="s">
-        <v>169</v>
-      </c>
+      <c r="D54" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E54" s="52"/>
       <c r="F54" s="53"/>
     </row>
-    <row r="55" spans="2:8">
+    <row r="55" spans="2:6">
       <c r="B55" s="60"/>
       <c r="C55" s="51"/>
       <c r="D55" s="52"/>
       <c r="E55" s="52" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="F55" s="53"/>
     </row>
-    <row r="56" spans="2:8">
+    <row r="56" spans="2:6">
       <c r="B56" s="60"/>
       <c r="C56" s="51"/>
       <c r="D56" s="52"/>
       <c r="E56" s="52" t="s">
-        <v>171</v>
+        <v>222</v>
       </c>
       <c r="F56" s="53"/>
     </row>
-    <row r="57" spans="2:8">
+    <row r="57" spans="2:6">
       <c r="B57" s="60"/>
       <c r="C57" s="51"/>
       <c r="D57" s="52"/>
       <c r="E57" s="52" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F57" s="53"/>
     </row>
-    <row r="58" spans="2:8">
+    <row r="58" spans="2:6">
       <c r="B58" s="60"/>
       <c r="C58" s="51"/>
       <c r="D58" s="52"/>
       <c r="E58" s="52" t="s">
-        <v>209</v>
+        <v>167</v>
       </c>
       <c r="F58" s="53"/>
-      <c r="H58" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8">
+    </row>
+    <row r="59" spans="2:6">
       <c r="B59" s="60"/>
       <c r="C59" s="51"/>
       <c r="D59" s="52"/>
@@ -5738,7 +5746,7 @@
       </c>
       <c r="F59" s="53"/>
     </row>
-    <row r="60" spans="2:8">
+    <row r="60" spans="2:6">
       <c r="B60" s="60"/>
       <c r="C60" s="51"/>
       <c r="D60" s="52"/>
@@ -5747,7 +5755,7 @@
       </c>
       <c r="F60" s="53"/>
     </row>
-    <row r="61" spans="2:8" ht="15.75" thickBot="1">
+    <row r="61" spans="2:6" ht="15.75" thickBot="1">
       <c r="B61" s="60"/>
       <c r="C61" s="54"/>
       <c r="D61" s="55"/>
@@ -5756,27 +5764,27 @@
       </c>
       <c r="F61" s="56"/>
     </row>
-    <row r="62" spans="2:8">
+    <row r="62" spans="2:6">
       <c r="B62" s="62" t="s">
-        <v>234</v>
-      </c>
-      <c r="C62" s="83" t="s">
-        <v>224</v>
+        <v>233</v>
+      </c>
+      <c r="C62" s="63" t="s">
+        <v>223</v>
       </c>
       <c r="D62" s="49"/>
       <c r="E62" s="49"/>
       <c r="F62" s="50"/>
     </row>
-    <row r="63" spans="2:8">
+    <row r="63" spans="2:6">
       <c r="B63" s="59"/>
       <c r="C63" s="51"/>
-      <c r="D63" s="86" t="s">
+      <c r="D63" s="66" t="s">
         <v>196</v>
       </c>
       <c r="E63" s="52"/>
       <c r="F63" s="53"/>
     </row>
-    <row r="64" spans="2:8">
+    <row r="64" spans="2:6">
       <c r="B64" s="59"/>
       <c r="C64" s="51"/>
       <c r="D64" s="52"/>
@@ -5790,7 +5798,7 @@
       <c r="C65" s="51"/>
       <c r="D65" s="52"/>
       <c r="E65" s="52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F65" s="53"/>
     </row>
@@ -5799,7 +5807,7 @@
       <c r="C66" s="51"/>
       <c r="D66" s="52"/>
       <c r="E66" s="52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F66" s="53"/>
     </row>
@@ -5808,7 +5816,7 @@
       <c r="C67" s="54"/>
       <c r="D67" s="55"/>
       <c r="E67" s="55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F67" s="56"/>
     </row>
@@ -5820,7 +5828,7 @@
     <row r="69" spans="2:6">
       <c r="B69" s="59"/>
       <c r="C69" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D69" s="49"/>
       <c r="E69" s="49"/>
@@ -5829,7 +5837,7 @@
     <row r="70" spans="2:6">
       <c r="B70" s="59"/>
       <c r="C70" s="51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D70" s="52"/>
       <c r="E70" s="52"/>
@@ -5838,7 +5846,7 @@
     <row r="71" spans="2:6">
       <c r="B71" s="59"/>
       <c r="C71" s="51" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D71" s="52"/>
       <c r="E71" s="52"/>
@@ -5877,7 +5885,7 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B1" t="s">
         <v>143</v>
@@ -5966,10 +5974,10 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="61" t="s">
         <v>235</v>
-      </c>
-      <c r="F7" s="61" t="s">
-        <v>236</v>
       </c>
       <c r="G7" s="61"/>
       <c r="H7" s="61"/>
@@ -5984,7 +5992,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="B8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F8" s="61"/>
       <c r="G8" s="61"/>
@@ -6000,10 +6008,10 @@
     </row>
     <row r="9" spans="1:16">
       <c r="B9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" s="61" t="s">
         <v>240</v>
-      </c>
-      <c r="F9" s="61" t="s">
-        <v>241</v>
       </c>
       <c r="G9" s="61"/>
       <c r="H9" s="61"/>
@@ -6082,13 +6090,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -6096,66 +6104,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="65" t="s">
+      <c r="K2" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="65" t="s">
+      <c r="Q2" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="67"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="71"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="74" t="s">
+      <c r="V2" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="76"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="80"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="77" t="s">
+      <c r="AA2" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="79"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="82"/>
+      <c r="AF2" s="82"/>
+      <c r="AG2" s="83"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="74" t="s">
+      <c r="AI2" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="75"/>
-      <c r="AP2" s="75"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="79"/>
+      <c r="AN2" s="79"/>
+      <c r="AO2" s="79"/>
+      <c r="AP2" s="79"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="82" t="s">
+      <c r="E3" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="84" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -6182,12 +6190,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="71"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Done SignUp Component (Membership Module)
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="245">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -1001,6 +1001,12 @@
   </si>
   <si>
     <t>bs-rating</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>IBsBreadcrumb</t>
   </si>
 </sst>
 </file>
@@ -1547,7 +1553,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1699,6 +1705,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2888,41 +2895,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="68" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67" t="s">
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -2930,66 +2937,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="79"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="76" t="s">
+      <c r="Q2" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="78"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="79"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="68" t="s">
+      <c r="V2" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="71"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="71" t="s">
+      <c r="AA2" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="72"/>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="74"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="68" t="s">
+      <c r="AI2" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="69"/>
-      <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
-      <c r="AM2" s="69"/>
-      <c r="AN2" s="69"/>
-      <c r="AO2" s="69"/>
-      <c r="AP2" s="69"/>
+      <c r="AJ2" s="70"/>
+      <c r="AK2" s="70"/>
+      <c r="AL2" s="70"/>
+      <c r="AM2" s="70"/>
+      <c r="AN2" s="70"/>
+      <c r="AO2" s="70"/>
+      <c r="AP2" s="70"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="75" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -3016,12 +3023,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="82"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>
@@ -5081,10 +5088,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T78"/>
+  <dimension ref="A2:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I39" activeCellId="1" sqref="G37 I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5143,10 +5150,13 @@
       <c r="B7" s="60"/>
       <c r="C7" s="51"/>
       <c r="D7" s="52"/>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="F7" s="53"/>
+      <c r="F7" s="65"/>
+      <c r="G7" t="s">
+        <v>243</v>
+      </c>
       <c r="S7" s="52"/>
     </row>
     <row r="8" spans="1:20">
@@ -5157,6 +5167,9 @@
         <v>208</v>
       </c>
       <c r="F8" s="65"/>
+      <c r="G8" t="s">
+        <v>243</v>
+      </c>
       <c r="N8" s="48" t="s">
         <v>150</v>
       </c>
@@ -5175,6 +5188,9 @@
         <v>236</v>
       </c>
       <c r="F9" s="65"/>
+      <c r="G9" t="s">
+        <v>243</v>
+      </c>
       <c r="N9" s="51"/>
       <c r="O9" s="52" t="s">
         <v>170</v>
@@ -5193,6 +5209,9 @@
         <v>242</v>
       </c>
       <c r="F10" s="65"/>
+      <c r="G10" t="s">
+        <v>243</v>
+      </c>
       <c r="H10" t="s">
         <v>209</v>
       </c>
@@ -5370,46 +5389,46 @@
       <c r="S19" s="55"/>
       <c r="T19" s="56"/>
     </row>
-    <row r="20" spans="2:20" ht="15.75" thickBot="1">
+    <row r="20" spans="2:20">
       <c r="B20" s="60"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55" t="s">
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52" t="s">
         <v>155</v>
       </c>
-      <c r="F20" s="56"/>
-    </row>
-    <row r="21" spans="2:20">
-      <c r="B21" s="62" t="s">
+      <c r="F20" s="53"/>
+    </row>
+    <row r="21" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B21" s="60"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="F21" s="56"/>
+    </row>
+    <row r="22" spans="2:20">
+      <c r="B22" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C21" s="63" t="s">
+      <c r="C22" s="67" t="s">
         <v>199</v>
       </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="50"/>
-      <c r="H21" s="61" t="s">
-        <v>228</v>
-      </c>
-      <c r="S21" s="52"/>
-    </row>
-    <row r="22" spans="2:20">
-      <c r="B22" s="60"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="66" t="s">
-        <v>196</v>
-      </c>
+      <c r="D22" s="52"/>
       <c r="E22" s="52"/>
       <c r="F22" s="53"/>
+      <c r="H22" s="61" t="s">
+        <v>228</v>
+      </c>
+      <c r="S22" s="52"/>
     </row>
     <row r="23" spans="2:20">
       <c r="B23" s="60"/>
       <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52" t="s">
-        <v>150</v>
-      </c>
+      <c r="D23" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E23" s="52"/>
       <c r="F23" s="53"/>
     </row>
     <row r="24" spans="2:20">
@@ -5417,7 +5436,7 @@
       <c r="C24" s="51"/>
       <c r="D24" s="52"/>
       <c r="E24" s="52" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F24" s="53"/>
     </row>
@@ -5426,7 +5445,7 @@
       <c r="C25" s="51"/>
       <c r="D25" s="52"/>
       <c r="E25" s="52" t="s">
-        <v>237</v>
+        <v>157</v>
       </c>
       <c r="F25" s="53"/>
     </row>
@@ -5435,7 +5454,7 @@
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
       <c r="E26" s="52" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="F26" s="53"/>
     </row>
@@ -5444,7 +5463,7 @@
       <c r="C27" s="51"/>
       <c r="D27" s="52"/>
       <c r="E27" s="52" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F27" s="53"/>
     </row>
@@ -5453,7 +5472,7 @@
       <c r="C28" s="51"/>
       <c r="D28" s="52"/>
       <c r="E28" s="52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F28" s="53"/>
     </row>
@@ -5462,185 +5481,188 @@
       <c r="C29" s="51"/>
       <c r="D29" s="52"/>
       <c r="E29" s="52" t="s">
+        <v>205</v>
+      </c>
+      <c r="F29" s="53"/>
+    </row>
+    <row r="30" spans="2:20">
+      <c r="B30" s="60"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="F29" s="53"/>
-    </row>
-    <row r="30" spans="2:20" ht="15.75" thickBot="1">
-      <c r="B30" s="60"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55" t="s">
+      <c r="F30" s="53"/>
+    </row>
+    <row r="31" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B31" s="60"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="F30" s="56"/>
-    </row>
-    <row r="31" spans="2:20">
-      <c r="B31" s="62" t="s">
+      <c r="F31" s="56"/>
+    </row>
+    <row r="32" spans="2:20">
+      <c r="B32" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C32" s="63" t="s">
         <v>198</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="50"/>
-      <c r="H31" s="61" t="s">
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="50"/>
+      <c r="H32" s="61" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="2:20">
-      <c r="B32" s="60"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E32" s="52"/>
-      <c r="F32" s="53"/>
-    </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:7">
       <c r="B33" s="60"/>
       <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52" t="s">
-        <v>151</v>
-      </c>
+      <c r="D33" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" s="52"/>
       <c r="F33" s="53"/>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:7">
       <c r="B34" s="60"/>
       <c r="C34" s="51"/>
       <c r="D34" s="52"/>
       <c r="E34" s="52" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="F34" s="53"/>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:7">
       <c r="B35" s="60"/>
       <c r="C35" s="51"/>
       <c r="D35" s="52"/>
       <c r="E35" s="52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F35" s="53"/>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:7">
       <c r="B36" s="60"/>
       <c r="C36" s="51"/>
       <c r="D36" s="52"/>
-      <c r="E36" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="F36" s="53"/>
-    </row>
-    <row r="37" spans="2:6">
+      <c r="E36" s="64" t="s">
+        <v>201</v>
+      </c>
+      <c r="F36" s="65"/>
+      <c r="G36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
       <c r="B37" s="60"/>
       <c r="C37" s="51"/>
       <c r="D37" s="52"/>
       <c r="E37" s="52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F37" s="53"/>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:7">
       <c r="B38" s="60"/>
       <c r="C38" s="51"/>
       <c r="D38" s="52"/>
       <c r="E38" s="52" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="F38" s="53"/>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:7">
       <c r="B39" s="60"/>
       <c r="C39" s="51"/>
       <c r="D39" s="52"/>
       <c r="E39" s="52" t="s">
-        <v>160</v>
+        <v>215</v>
       </c>
       <c r="F39" s="53"/>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:7">
       <c r="B40" s="60"/>
       <c r="C40" s="51"/>
       <c r="D40" s="52"/>
       <c r="E40" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F40" s="53"/>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:7">
       <c r="B41" s="60"/>
       <c r="C41" s="51"/>
       <c r="D41" s="52"/>
       <c r="E41" s="52" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F41" s="53"/>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:7">
       <c r="B42" s="60"/>
       <c r="C42" s="51"/>
       <c r="D42" s="52"/>
       <c r="E42" s="52" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F42" s="53"/>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:7">
       <c r="B43" s="60"/>
       <c r="C43" s="51"/>
-      <c r="D43" s="66" t="s">
+      <c r="D43" s="52"/>
+      <c r="E43" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" s="53"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="60"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="66" t="s">
         <v>216</v>
       </c>
-      <c r="E43" s="52"/>
-      <c r="F43" s="53"/>
-    </row>
-    <row r="44" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B44" s="60"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55" t="s">
+      <c r="E44" s="52"/>
+      <c r="F44" s="53"/>
+    </row>
+    <row r="45" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B45" s="60"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="F44" s="56"/>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="B45" s="62" t="s">
+      <c r="F45" s="56"/>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="63" t="s">
+      <c r="C46" s="63" t="s">
         <v>213</v>
       </c>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="50"/>
-    </row>
-    <row r="46" spans="2:6">
-      <c r="B46" s="60"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E46" s="52"/>
-      <c r="F46" s="53"/>
-    </row>
-    <row r="47" spans="2:6">
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="50"/>
+    </row>
+    <row r="47" spans="2:7">
       <c r="B47" s="60"/>
       <c r="C47" s="51"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="52" t="s">
-        <v>217</v>
-      </c>
+      <c r="D47" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E47" s="52"/>
       <c r="F47" s="53"/>
     </row>
-    <row r="48" spans="2:6">
+    <row r="48" spans="2:7">
       <c r="B48" s="60"/>
       <c r="C48" s="51"/>
       <c r="D48" s="52"/>
       <c r="E48" s="52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F48" s="53"/>
     </row>
@@ -5649,7 +5671,7 @@
       <c r="C49" s="51"/>
       <c r="D49" s="52"/>
       <c r="E49" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F49" s="53"/>
     </row>
@@ -5658,55 +5680,55 @@
       <c r="C50" s="51"/>
       <c r="D50" s="52"/>
       <c r="E50" s="52" t="s">
-        <v>162</v>
+        <v>219</v>
       </c>
       <c r="F50" s="53"/>
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="60"/>
       <c r="C51" s="51"/>
-      <c r="D51" s="66" t="s">
+      <c r="D51" s="52"/>
+      <c r="E51" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="F51" s="53"/>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="60"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="E51" s="52"/>
-      <c r="F51" s="53"/>
-    </row>
-    <row r="52" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B52" s="60"/>
-      <c r="C52" s="54"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55" t="s">
+      <c r="E52" s="52"/>
+      <c r="F52" s="53"/>
+    </row>
+    <row r="53" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B53" s="60"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="F52" s="56"/>
-    </row>
-    <row r="53" spans="2:6">
-      <c r="B53" s="62" t="s">
+      <c r="F53" s="56"/>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="C53" s="63" t="s">
+      <c r="C54" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="D53" s="49"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="50"/>
-    </row>
-    <row r="54" spans="2:6">
-      <c r="B54" s="60"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E54" s="52"/>
-      <c r="F54" s="53"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="50"/>
     </row>
     <row r="55" spans="2:6">
       <c r="B55" s="60"/>
       <c r="C55" s="51"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52" t="s">
-        <v>169</v>
-      </c>
+      <c r="D55" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E55" s="52"/>
       <c r="F55" s="53"/>
     </row>
     <row r="56" spans="2:6">
@@ -5714,7 +5736,7 @@
       <c r="C56" s="51"/>
       <c r="D56" s="52"/>
       <c r="E56" s="52" t="s">
-        <v>222</v>
+        <v>169</v>
       </c>
       <c r="F56" s="53"/>
     </row>
@@ -5723,7 +5745,7 @@
       <c r="C57" s="51"/>
       <c r="D57" s="52"/>
       <c r="E57" s="52" t="s">
-        <v>171</v>
+        <v>222</v>
       </c>
       <c r="F57" s="53"/>
     </row>
@@ -5732,7 +5754,7 @@
       <c r="C58" s="51"/>
       <c r="D58" s="52"/>
       <c r="E58" s="52" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F58" s="53"/>
     </row>
@@ -5741,7 +5763,7 @@
       <c r="C59" s="51"/>
       <c r="D59" s="52"/>
       <c r="E59" s="52" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="F59" s="53"/>
     </row>
@@ -5750,46 +5772,46 @@
       <c r="C60" s="51"/>
       <c r="D60" s="52"/>
       <c r="E60" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="F60" s="53"/>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="B61" s="60"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="52"/>
+      <c r="E61" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="F60" s="53"/>
-    </row>
-    <row r="61" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B61" s="60"/>
-      <c r="C61" s="54"/>
-      <c r="D61" s="55"/>
-      <c r="E61" s="55" t="s">
+      <c r="F61" s="53"/>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B62" s="60"/>
+      <c r="C62" s="54"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="F61" s="56"/>
-    </row>
-    <row r="62" spans="2:6">
-      <c r="B62" s="62" t="s">
+      <c r="F62" s="56"/>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C62" s="63" t="s">
+      <c r="C63" s="63" t="s">
         <v>223</v>
       </c>
-      <c r="D62" s="49"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="50"/>
-    </row>
-    <row r="63" spans="2:6">
-      <c r="B63" s="59"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E63" s="52"/>
-      <c r="F63" s="53"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="50"/>
     </row>
     <row r="64" spans="2:6">
       <c r="B64" s="59"/>
       <c r="C64" s="51"/>
-      <c r="D64" s="52"/>
-      <c r="E64" s="52" t="s">
-        <v>164</v>
-      </c>
+      <c r="D64" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E64" s="52"/>
       <c r="F64" s="53"/>
     </row>
     <row r="65" spans="2:6">
@@ -5797,7 +5819,7 @@
       <c r="C65" s="51"/>
       <c r="D65" s="52"/>
       <c r="E65" s="52" t="s">
-        <v>224</v>
+        <v>164</v>
       </c>
       <c r="F65" s="53"/>
     </row>
@@ -5806,65 +5828,74 @@
       <c r="C66" s="51"/>
       <c r="D66" s="52"/>
       <c r="E66" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="F66" s="53"/>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="59"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="F66" s="53"/>
-    </row>
-    <row r="67" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B67" s="59"/>
-      <c r="C67" s="54"/>
-      <c r="D67" s="55"/>
-      <c r="E67" s="55" t="s">
+      <c r="F67" s="53"/>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B68" s="59"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="F67" s="56"/>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B68" s="58" t="s">
+      <c r="F68" s="56"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B69" s="58" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="69" spans="2:6">
-      <c r="B69" s="59"/>
-      <c r="C69" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D69" s="49"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="50"/>
     </row>
     <row r="70" spans="2:6">
       <c r="B70" s="59"/>
-      <c r="C70" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="D70" s="52"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="53"/>
+      <c r="C70" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="D70" s="49"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="50"/>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" s="59"/>
       <c r="C71" s="51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D71" s="52"/>
       <c r="E71" s="52"/>
       <c r="F71" s="53"/>
     </row>
-    <row r="72" spans="2:6" ht="15.75" thickBot="1">
+    <row r="72" spans="2:6">
       <c r="B72" s="59"/>
-      <c r="C72" s="54"/>
-      <c r="D72" s="55"/>
-      <c r="E72" s="55"/>
-      <c r="F72" s="56"/>
-    </row>
-    <row r="73" spans="2:6">
-      <c r="B73" s="58" t="s">
+      <c r="C72" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="D72" s="52"/>
+      <c r="E72" s="52"/>
+      <c r="F72" s="53"/>
+    </row>
+    <row r="73" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B73" s="59"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="55"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="56"/>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="2:6">
-      <c r="B78" s="59"/>
+    <row r="79" spans="2:6">
+      <c r="B79" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6089,13 +6120,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -6103,66 +6134,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="79"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="76" t="s">
+      <c r="Q2" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="78"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="79"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="68" t="s">
+      <c r="V2" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="71"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="71" t="s">
+      <c r="AA2" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="72"/>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="74"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="68" t="s">
+      <c r="AI2" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="69"/>
-      <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
-      <c r="AM2" s="69"/>
-      <c r="AN2" s="69"/>
-      <c r="AO2" s="69"/>
-      <c r="AP2" s="69"/>
+      <c r="AJ2" s="70"/>
+      <c r="AK2" s="70"/>
+      <c r="AL2" s="70"/>
+      <c r="AM2" s="70"/>
+      <c r="AN2" s="70"/>
+      <c r="AO2" s="70"/>
+      <c r="AP2" s="70"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="D3" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="85" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -6189,12 +6220,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="82"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
fix bug bs-nav height=0, add admin page
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENT\HK6\TTTN\iFoody\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOCUMENT\TTTN\iFoody\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="247">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -1008,11 +1008,17 @@
   <si>
     <t>IBsBreadcrumb</t>
   </si>
+  <si>
+    <t>for user open store</t>
+  </si>
+  <si>
+    <t>admin-page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="34">
     <font>
       <sz val="11"/>
@@ -1259,7 +1265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1310,6 +1316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1553,7 +1565,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1705,7 +1717,36 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1727,36 +1768,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1766,6 +1777,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="% complete" xfId="12"/>
@@ -2895,41 +2917,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68" t="s">
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -2937,66 +2959,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="77" t="s">
+      <c r="K2" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="79"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="77" t="s">
+      <c r="Q2" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="79"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="71"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="69" t="s">
+      <c r="V2" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="71"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="80"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="72" t="s">
+      <c r="AA2" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="74"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="82"/>
+      <c r="AF2" s="82"/>
+      <c r="AG2" s="83"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="69" t="s">
+      <c r="AI2" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="70"/>
-      <c r="AK2" s="70"/>
-      <c r="AL2" s="70"/>
-      <c r="AM2" s="70"/>
-      <c r="AN2" s="70"/>
-      <c r="AO2" s="70"/>
-      <c r="AP2" s="70"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="79"/>
+      <c r="AN2" s="79"/>
+      <c r="AO2" s="79"/>
+      <c r="AP2" s="79"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="G3" s="67" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -3023,12 +3045,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="83"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>
@@ -4903,6 +4925,11 @@
     <row r="31" spans="2:52" ht="30" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:AB1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
@@ -4912,11 +4939,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:AB1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AI2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="BA5:BO30">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -5088,10 +5110,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T79"/>
+  <dimension ref="A2:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5411,12 +5433,12 @@
       <c r="B22" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="87" t="s">
         <v>199</v>
       </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="53"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="89"/>
       <c r="H22" s="61" t="s">
         <v>228</v>
       </c>
@@ -5424,96 +5446,96 @@
     </row>
     <row r="23" spans="2:20">
       <c r="B23" s="60"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="66" t="s">
+      <c r="C23" s="90"/>
+      <c r="D23" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="E23" s="52"/>
-      <c r="F23" s="53"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="89"/>
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="60"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52" t="s">
+      <c r="C24" s="90"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="F24" s="53"/>
+      <c r="F24" s="89"/>
       <c r="G24" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="25" spans="2:20">
       <c r="B25" s="60"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52" t="s">
+      <c r="C25" s="90"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="53"/>
+      <c r="F25" s="89"/>
       <c r="G25" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="26" spans="2:20">
       <c r="B26" s="60"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52" t="s">
+      <c r="C26" s="90"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="88" t="s">
         <v>237</v>
       </c>
-      <c r="F26" s="53"/>
+      <c r="F26" s="89"/>
       <c r="G26" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="27" spans="2:20">
       <c r="B27" s="60"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52" t="s">
+      <c r="C27" s="90"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88" t="s">
         <v>197</v>
       </c>
-      <c r="F27" s="53"/>
+      <c r="F27" s="89"/>
       <c r="G27" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="28" spans="2:20">
       <c r="B28" s="60"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52" t="s">
+      <c r="C28" s="90"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88" t="s">
         <v>204</v>
       </c>
-      <c r="F28" s="53"/>
+      <c r="F28" s="89"/>
     </row>
     <row r="29" spans="2:20">
       <c r="B29" s="60"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52" t="s">
+      <c r="C29" s="90"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88" t="s">
         <v>205</v>
       </c>
-      <c r="F29" s="53"/>
+      <c r="F29" s="89"/>
     </row>
     <row r="30" spans="2:20">
       <c r="B30" s="60"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52" t="s">
+      <c r="C30" s="90"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88" t="s">
         <v>206</v>
       </c>
-      <c r="F30" s="53"/>
+      <c r="F30" s="89"/>
     </row>
     <row r="31" spans="2:20" ht="15.75" thickBot="1">
       <c r="B31" s="60"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55" t="s">
+      <c r="C31" s="92"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="94"/>
     </row>
     <row r="32" spans="2:20">
       <c r="B32" s="62" t="s">
@@ -5653,261 +5675,273 @@
       <c r="B46" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C46" s="63" t="s">
+      <c r="C46" s="95" t="s">
         <v>213</v>
       </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="50"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="97"/>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="60"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="66" t="s">
+      <c r="C47" s="90"/>
+      <c r="D47" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="E47" s="52"/>
-      <c r="F47" s="53"/>
+      <c r="E47" s="88"/>
+      <c r="F47" s="89"/>
     </row>
     <row r="48" spans="2:7">
       <c r="B48" s="60"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52" t="s">
+      <c r="C48" s="90"/>
+      <c r="D48" s="91"/>
+      <c r="E48" s="88" t="s">
+        <v>246</v>
+      </c>
+      <c r="F48" s="89"/>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" s="60"/>
+      <c r="C49" s="90"/>
+      <c r="D49" s="88"/>
+      <c r="E49" s="88" t="s">
         <v>217</v>
       </c>
-      <c r="F48" s="53"/>
-    </row>
-    <row r="49" spans="2:6">
-      <c r="B49" s="60"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="52" t="s">
+      <c r="F49" s="89"/>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="60"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="F49" s="53"/>
-    </row>
-    <row r="50" spans="2:6">
-      <c r="B50" s="60"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52" t="s">
+      <c r="F50" s="89"/>
+    </row>
+    <row r="51" spans="2:7">
+      <c r="B51" s="60"/>
+      <c r="C51" s="90"/>
+      <c r="D51" s="88"/>
+      <c r="E51" s="88" t="s">
         <v>219</v>
       </c>
-      <c r="F50" s="53"/>
-    </row>
-    <row r="51" spans="2:6">
-      <c r="B51" s="60"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="52" t="s">
+      <c r="F51" s="89"/>
+      <c r="G51" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52" s="60"/>
+      <c r="C52" s="90"/>
+      <c r="D52" s="88"/>
+      <c r="E52" s="88" t="s">
         <v>162</v>
       </c>
-      <c r="F51" s="53"/>
-    </row>
-    <row r="52" spans="2:6">
-      <c r="B52" s="60"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="66" t="s">
+      <c r="F52" s="89"/>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" s="60"/>
+      <c r="C53" s="90"/>
+      <c r="D53" s="91" t="s">
         <v>188</v>
       </c>
-      <c r="E52" s="52"/>
-      <c r="F52" s="53"/>
-    </row>
-    <row r="53" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B53" s="60"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55" t="s">
+      <c r="E53" s="88"/>
+      <c r="F53" s="89"/>
+    </row>
+    <row r="54" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B54" s="60"/>
+      <c r="C54" s="92"/>
+      <c r="D54" s="93"/>
+      <c r="E54" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="F53" s="56"/>
-    </row>
-    <row r="54" spans="2:6">
-      <c r="B54" s="62" t="s">
+      <c r="F54" s="94"/>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="C54" s="63" t="s">
+      <c r="C55" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="D54" s="49"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="50"/>
-    </row>
-    <row r="55" spans="2:6">
-      <c r="B55" s="60"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E55" s="52"/>
-      <c r="F55" s="53"/>
-    </row>
-    <row r="56" spans="2:6">
+      <c r="D55" s="49"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="50"/>
+    </row>
+    <row r="56" spans="2:7">
       <c r="B56" s="60"/>
       <c r="C56" s="51"/>
-      <c r="D56" s="52"/>
-      <c r="E56" s="52" t="s">
-        <v>169</v>
-      </c>
+      <c r="D56" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E56" s="52"/>
       <c r="F56" s="53"/>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:7">
       <c r="B57" s="60"/>
       <c r="C57" s="51"/>
       <c r="D57" s="52"/>
       <c r="E57" s="52" t="s">
-        <v>222</v>
+        <v>169</v>
       </c>
       <c r="F57" s="53"/>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:7">
       <c r="B58" s="60"/>
       <c r="C58" s="51"/>
       <c r="D58" s="52"/>
       <c r="E58" s="52" t="s">
-        <v>171</v>
+        <v>222</v>
       </c>
       <c r="F58" s="53"/>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:7">
       <c r="B59" s="60"/>
       <c r="C59" s="51"/>
       <c r="D59" s="52"/>
       <c r="E59" s="52" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F59" s="53"/>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:7">
       <c r="B60" s="60"/>
       <c r="C60" s="51"/>
       <c r="D60" s="52"/>
       <c r="E60" s="52" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="F60" s="53"/>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="2:7">
       <c r="B61" s="60"/>
       <c r="C61" s="51"/>
       <c r="D61" s="52"/>
       <c r="E61" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="F61" s="53"/>
+    </row>
+    <row r="62" spans="2:7">
+      <c r="B62" s="60"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="F61" s="53"/>
-    </row>
-    <row r="62" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B62" s="60"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55" t="s">
+      <c r="F62" s="53"/>
+    </row>
+    <row r="63" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B63" s="60"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="F62" s="56"/>
-    </row>
-    <row r="63" spans="2:6">
-      <c r="B63" s="62" t="s">
+      <c r="F63" s="56"/>
+    </row>
+    <row r="64" spans="2:7">
+      <c r="B64" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C63" s="63" t="s">
+      <c r="C64" s="95" t="s">
         <v>223</v>
       </c>
-      <c r="D63" s="49"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="50"/>
-    </row>
-    <row r="64" spans="2:6">
-      <c r="B64" s="59"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E64" s="52"/>
-      <c r="F64" s="53"/>
+      <c r="D64" s="96"/>
+      <c r="E64" s="96"/>
+      <c r="F64" s="97"/>
     </row>
     <row r="65" spans="2:6">
       <c r="B65" s="59"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="F65" s="53"/>
+      <c r="C65" s="90"/>
+      <c r="D65" s="91" t="s">
+        <v>196</v>
+      </c>
+      <c r="E65" s="88"/>
+      <c r="F65" s="89"/>
     </row>
     <row r="66" spans="2:6">
       <c r="B66" s="59"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="52"/>
-      <c r="E66" s="52" t="s">
-        <v>224</v>
-      </c>
-      <c r="F66" s="53"/>
+      <c r="C66" s="90"/>
+      <c r="D66" s="88"/>
+      <c r="E66" s="88" t="s">
+        <v>164</v>
+      </c>
+      <c r="F66" s="89"/>
     </row>
     <row r="67" spans="2:6">
       <c r="B67" s="59"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="52"/>
-      <c r="E67" s="52" t="s">
+      <c r="C67" s="90"/>
+      <c r="D67" s="88"/>
+      <c r="E67" s="88" t="s">
+        <v>224</v>
+      </c>
+      <c r="F67" s="89"/>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="59"/>
+      <c r="C68" s="90"/>
+      <c r="D68" s="88"/>
+      <c r="E68" s="88" t="s">
         <v>225</v>
       </c>
-      <c r="F67" s="53"/>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B68" s="59"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="55"/>
-      <c r="E68" s="55" t="s">
+      <c r="F68" s="89"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B69" s="59"/>
+      <c r="C69" s="92"/>
+      <c r="D69" s="93"/>
+      <c r="E69" s="93" t="s">
         <v>226</v>
       </c>
-      <c r="F68" s="56"/>
-    </row>
-    <row r="69" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B69" s="58" t="s">
+      <c r="F69" s="94"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B70" s="58" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="70" spans="2:6">
-      <c r="B70" s="59"/>
-      <c r="C70" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="50"/>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" s="59"/>
-      <c r="C71" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="D71" s="52"/>
-      <c r="E71" s="52"/>
-      <c r="F71" s="53"/>
+      <c r="C71" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" s="49"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="50"/>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" s="59"/>
       <c r="C72" s="51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D72" s="52"/>
       <c r="E72" s="52"/>
       <c r="F72" s="53"/>
     </row>
-    <row r="73" spans="2:6" ht="15.75" thickBot="1">
+    <row r="73" spans="2:6">
       <c r="B73" s="59"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="55"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="56"/>
-    </row>
-    <row r="74" spans="2:6">
-      <c r="B74" s="58" t="s">
+      <c r="C73" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="F73" s="53"/>
+    </row>
+    <row r="74" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B74" s="59"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="56"/>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="79" spans="2:6">
-      <c r="B79" s="59"/>
+    <row r="80" spans="2:6">
+      <c r="B80" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6132,13 +6166,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -6146,66 +6180,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="77" t="s">
+      <c r="K2" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="79"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="77" t="s">
+      <c r="Q2" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="79"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="71"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="69" t="s">
+      <c r="V2" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="71"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="80"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="72" t="s">
+      <c r="AA2" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="74"/>
+      <c r="AB2" s="82"/>
+      <c r="AC2" s="82"/>
+      <c r="AD2" s="82"/>
+      <c r="AE2" s="82"/>
+      <c r="AF2" s="82"/>
+      <c r="AG2" s="83"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="69" t="s">
+      <c r="AI2" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="70"/>
-      <c r="AK2" s="70"/>
-      <c r="AL2" s="70"/>
-      <c r="AM2" s="70"/>
-      <c r="AN2" s="70"/>
-      <c r="AO2" s="70"/>
-      <c r="AP2" s="70"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="79"/>
+      <c r="AN2" s="79"/>
+      <c r="AO2" s="79"/>
+      <c r="AP2" s="79"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="84" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -6232,12 +6266,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="83"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Done Login Component (Membership Module)
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENT\HK6\TTTN\iFoody\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\DAI HOC\HK5\TTTN\iFoody\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -19,28 +19,29 @@
     <sheet name="Note Teacher" sheetId="7" r:id="rId5"/>
     <sheet name="Note Project" sheetId="8" r:id="rId6"/>
     <sheet name="Note Tuấn" sheetId="9" r:id="rId7"/>
-    <sheet name="Project Planner (sample)" sheetId="5" state="hidden" r:id="rId8"/>
+    <sheet name="TIP" sheetId="10" r:id="rId8"/>
+    <sheet name="Project Planner (sample)" sheetId="5" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="Actual" localSheetId="7">('Project Planner (sample)'!PeriodInActual*('Project Planner (sample)'!$E1&gt;0))*'Project Planner (sample)'!PeriodInPlan</definedName>
+    <definedName name="Actual" localSheetId="8">('Project Planner (sample)'!PeriodInActual*('Project Planner (sample)'!$E1&gt;0))*'Project Planner (sample)'!PeriodInPlan</definedName>
     <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
-    <definedName name="ActualBeyond" localSheetId="7">'Project Planner (sample)'!PeriodInActual*('Project Planner (sample)'!$E1&gt;0)</definedName>
+    <definedName name="ActualBeyond" localSheetId="8">'Project Planner (sample)'!PeriodInActual*('Project Planner (sample)'!$E1&gt;0)</definedName>
     <definedName name="ActualBeyond">PeriodInActual*('Project Planner'!$E1&gt;0)</definedName>
-    <definedName name="PercentComplete" localSheetId="7">'Project Planner (sample)'!PercentCompleteBeyond*'Project Planner (sample)'!PeriodInPlan</definedName>
+    <definedName name="PercentComplete" localSheetId="8">'Project Planner (sample)'!PercentCompleteBeyond*'Project Planner (sample)'!PeriodInPlan</definedName>
     <definedName name="PercentComplete">PercentCompleteBeyond*PeriodInPlan</definedName>
-    <definedName name="PercentCompleteBeyond" localSheetId="7">('Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$E1,'Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1)*('Project Planner (sample)'!$E1&gt;0))*(('Project Planner (sample)'!A$4&lt;(INT('Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1*'Project Planner (sample)'!$G1)))+('Project Planner (sample)'!A$4='Project Planner (sample)'!$E1))*('Project Planner (sample)'!$G1&gt;0)</definedName>
+    <definedName name="PercentCompleteBeyond" localSheetId="8">('Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$E1,'Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1)*('Project Planner (sample)'!$E1&gt;0))*(('Project Planner (sample)'!A$4&lt;(INT('Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1*'Project Planner (sample)'!$G1)))+('Project Planner (sample)'!A$4='Project Planner (sample)'!$E1))*('Project Planner (sample)'!$G1&gt;0)</definedName>
     <definedName name="PercentCompleteBeyond">('Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1)*('Project Planner'!$E1&gt;0))*(('Project Planner'!A$4&lt;(INT('Project Planner'!$E1+'Project Planner'!$F1*'Project Planner'!$G1)))+('Project Planner'!A$4='Project Planner'!$E1))*('Project Planner'!$G1&gt;0)</definedName>
-    <definedName name="period_selected" localSheetId="7">'Project Planner (sample)'!$H$2</definedName>
+    <definedName name="period_selected" localSheetId="8">'Project Planner (sample)'!$H$2</definedName>
     <definedName name="period_selected">'Project Planner'!$H$2</definedName>
-    <definedName name="PeriodInActual" localSheetId="7">'Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$E1,'Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1-1)</definedName>
+    <definedName name="PeriodInActual" localSheetId="8">'Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$E1,'Project Planner (sample)'!$E1+'Project Planner (sample)'!$F1-1)</definedName>
     <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1-1)</definedName>
-    <definedName name="PeriodInPlan" localSheetId="7">'Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$C1,'Project Planner (sample)'!$C1+'Project Planner (sample)'!$D1-1)</definedName>
+    <definedName name="PeriodInPlan" localSheetId="8">'Project Planner (sample)'!A$4=MEDIAN('Project Planner (sample)'!A$4,'Project Planner (sample)'!$C1,'Project Planner (sample)'!$C1+'Project Planner (sample)'!$D1-1)</definedName>
     <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$C1,'Project Planner'!$C1+'Project Planner'!$D1-1)</definedName>
-    <definedName name="Plan" localSheetId="7">'Project Planner (sample)'!PeriodInPlan*('Project Planner (sample)'!$C1&gt;0)</definedName>
+    <definedName name="Plan" localSheetId="8">'Project Planner (sample)'!PeriodInPlan*('Project Planner (sample)'!$C1&gt;0)</definedName>
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Project Planner'!$3:$4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'Project Planner (sample)'!$3:$4</definedName>
-    <definedName name="TitleRegion..BO60" localSheetId="7">'Project Planner (sample)'!$B$3:$B$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">'Project Planner (sample)'!$3:$4</definedName>
+    <definedName name="TitleRegion..BO60" localSheetId="8">'Project Planner (sample)'!$B$3:$B$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="254">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -1008,12 +1009,39 @@
   <si>
     <t>IBsBreadcrumb</t>
   </si>
+  <si>
+    <t>airbnb</t>
+  </si>
+  <si>
+    <t>Tip:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set style cho thẻ component --&gt; sử dụng  :host trong scss ví dụ như     :host {color:  grey}    </t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Typescript (TS file)</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Dùng    btn-lg , input-lg    để set kích thước cho các các element trong bootstrap</t>
+  </si>
+  <si>
+    <t>profile (general page)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="34">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1258,8 +1286,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1310,6 +1346,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor theme="7"/>
+        <bgColor theme="5" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF96DE8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1553,7 +1619,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1706,6 +1772,14 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1766,6 +1840,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="% complete" xfId="12"/>
@@ -2078,6 +2154,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF96DE8"/>
       <color rgb="FFEC7524"/>
     </mruColors>
   </colors>
@@ -2361,7 +2438,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
@@ -2441,7 +2518,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15">
+    <row r="18" spans="1:13">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>54</v>
@@ -2550,7 +2627,7 @@
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -2565,7 +2642,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18.75">
+    <row r="3" spans="1:1" ht="19.5">
       <c r="A3" s="30" t="s">
         <v>80</v>
       </c>
@@ -2608,7 +2685,7 @@
     <row r="11" spans="1:1">
       <c r="A11" s="27"/>
     </row>
-    <row r="12" spans="1:1" ht="20.25">
+    <row r="12" spans="1:1" ht="21">
       <c r="A12" s="30" t="s">
         <v>81</v>
       </c>
@@ -2636,7 +2713,7 @@
     <row r="17" spans="1:1">
       <c r="A17" s="28"/>
     </row>
-    <row r="18" spans="1:1" ht="20.25">
+    <row r="18" spans="1:1" ht="21">
       <c r="A18" s="30" t="s">
         <v>82</v>
       </c>
@@ -2659,7 +2736,7 @@
     <row r="22" spans="1:1">
       <c r="A22" s="29"/>
     </row>
-    <row r="23" spans="1:1" ht="20.25">
+    <row r="23" spans="1:1" ht="21">
       <c r="A23" s="30" t="s">
         <v>83</v>
       </c>
@@ -2873,8 +2950,8 @@
   </sheetPr>
   <dimension ref="B1:BO31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="30" customHeight="1"/>
@@ -2895,41 +2972,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="78" t="s">
+      <c r="G1" s="84" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78" t="s">
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -2937,66 +3014,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="70" t="s">
+      <c r="K2" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="70" t="s">
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="72"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="78"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="79" t="s">
+      <c r="V2" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="80"/>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="81"/>
+      <c r="W2" s="86"/>
+      <c r="X2" s="86"/>
+      <c r="Y2" s="87"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="82" t="s">
+      <c r="AA2" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="83"/>
-      <c r="AC2" s="83"/>
-      <c r="AD2" s="83"/>
-      <c r="AE2" s="83"/>
-      <c r="AF2" s="83"/>
-      <c r="AG2" s="84"/>
+      <c r="AB2" s="89"/>
+      <c r="AC2" s="89"/>
+      <c r="AD2" s="89"/>
+      <c r="AE2" s="89"/>
+      <c r="AF2" s="89"/>
+      <c r="AG2" s="90"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="79" t="s">
+      <c r="AI2" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="80"/>
-      <c r="AK2" s="80"/>
-      <c r="AL2" s="80"/>
-      <c r="AM2" s="80"/>
-      <c r="AN2" s="80"/>
-      <c r="AO2" s="80"/>
-      <c r="AP2" s="80"/>
-    </row>
-    <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="75" t="s">
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="86"/>
+      <c r="AL2" s="86"/>
+      <c r="AM2" s="86"/>
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="86"/>
+      <c r="AP2" s="86"/>
+    </row>
+    <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B3" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="74" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -3022,23 +3099,23 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="76"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="9">
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B4" s="82"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="16">
         <v>1</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="16">
         <v>2</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="16">
         <v>3</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="17">
         <v>4</v>
       </c>
       <c r="L4" s="9">
@@ -3426,8 +3503,8 @@
       </c>
       <c r="H8"/>
       <c r="I8"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="18"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="68"/>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8"/>
@@ -4949,9 +5026,9 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:BO4">
+  <conditionalFormatting sqref="L4:BO4">
     <cfRule type="expression" dxfId="10" priority="8">
-      <formula>H$4=period_selected</formula>
+      <formula>L$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
@@ -5088,10 +5165,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T79"/>
+  <dimension ref="A2:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5151,7 +5228,7 @@
       <c r="C7" s="51"/>
       <c r="D7" s="52"/>
       <c r="E7" s="64" t="s">
-        <v>154</v>
+        <v>245</v>
       </c>
       <c r="F7" s="65"/>
       <c r="G7" t="s">
@@ -5435,10 +5512,10 @@
       <c r="B24" s="60"/>
       <c r="C24" s="51"/>
       <c r="D24" s="52"/>
-      <c r="E24" s="52" t="s">
+      <c r="E24" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="F24" s="53"/>
+      <c r="F24" s="65"/>
       <c r="G24" t="s">
         <v>243</v>
       </c>
@@ -5447,10 +5524,10 @@
       <c r="B25" s="60"/>
       <c r="C25" s="51"/>
       <c r="D25" s="52"/>
-      <c r="E25" s="52" t="s">
+      <c r="E25" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="53"/>
+      <c r="F25" s="65"/>
       <c r="G25" t="s">
         <v>243</v>
       </c>
@@ -5459,10 +5536,10 @@
       <c r="B26" s="60"/>
       <c r="C26" s="51"/>
       <c r="D26" s="52"/>
-      <c r="E26" s="52" t="s">
+      <c r="E26" s="64" t="s">
         <v>237</v>
       </c>
-      <c r="F26" s="53"/>
+      <c r="F26" s="65"/>
       <c r="G26" t="s">
         <v>243</v>
       </c>
@@ -5539,10 +5616,13 @@
       <c r="B34" s="60"/>
       <c r="C34" s="51"/>
       <c r="D34" s="52"/>
-      <c r="E34" s="52" t="s">
+      <c r="E34" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="53"/>
+      <c r="F34" s="65"/>
+      <c r="G34" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="60"/>
@@ -5569,17 +5649,17 @@
       <c r="B37" s="60"/>
       <c r="C37" s="51"/>
       <c r="D37" s="52"/>
-      <c r="E37" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="F37" s="95"/>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="60"/>
       <c r="C38" s="51"/>
       <c r="D38" s="52"/>
       <c r="E38" s="52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F38" s="53"/>
     </row>
@@ -5588,7 +5668,7 @@
       <c r="C39" s="51"/>
       <c r="D39" s="52"/>
       <c r="E39" s="52" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="F39" s="53"/>
     </row>
@@ -5597,7 +5677,7 @@
       <c r="C40" s="51"/>
       <c r="D40" s="52"/>
       <c r="E40" s="52" t="s">
-        <v>160</v>
+        <v>215</v>
       </c>
       <c r="F40" s="53"/>
     </row>
@@ -5606,7 +5686,7 @@
       <c r="C41" s="51"/>
       <c r="D41" s="52"/>
       <c r="E41" s="52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F41" s="53"/>
     </row>
@@ -5615,7 +5695,7 @@
       <c r="C42" s="51"/>
       <c r="D42" s="52"/>
       <c r="E42" s="52" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F42" s="53"/>
     </row>
@@ -5624,55 +5704,55 @@
       <c r="C43" s="51"/>
       <c r="D43" s="52"/>
       <c r="E43" s="52" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="F43" s="53"/>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" s="60"/>
       <c r="C44" s="51"/>
-      <c r="D44" s="66" t="s">
+      <c r="D44" s="52"/>
+      <c r="E44" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="F44" s="53"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="60"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="66" t="s">
         <v>216</v>
       </c>
-      <c r="E44" s="52"/>
-      <c r="F44" s="53"/>
-    </row>
-    <row r="45" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B45" s="60"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55" t="s">
+      <c r="E45" s="52"/>
+      <c r="F45" s="53"/>
+    </row>
+    <row r="46" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B46" s="60"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="F45" s="56"/>
-    </row>
-    <row r="46" spans="2:7">
-      <c r="B46" s="62" t="s">
+      <c r="F46" s="56"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C46" s="63" t="s">
+      <c r="C47" s="63" t="s">
         <v>213</v>
       </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="50"/>
-    </row>
-    <row r="47" spans="2:7">
-      <c r="B47" s="60"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E47" s="52"/>
-      <c r="F47" s="53"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="50"/>
     </row>
     <row r="48" spans="2:7">
       <c r="B48" s="60"/>
       <c r="C48" s="51"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52" t="s">
-        <v>217</v>
-      </c>
+      <c r="D48" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E48" s="52"/>
       <c r="F48" s="53"/>
     </row>
     <row r="49" spans="2:6">
@@ -5680,7 +5760,7 @@
       <c r="C49" s="51"/>
       <c r="D49" s="52"/>
       <c r="E49" s="52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F49" s="53"/>
     </row>
@@ -5689,7 +5769,7 @@
       <c r="C50" s="51"/>
       <c r="D50" s="52"/>
       <c r="E50" s="52" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F50" s="53"/>
     </row>
@@ -5698,55 +5778,55 @@
       <c r="C51" s="51"/>
       <c r="D51" s="52"/>
       <c r="E51" s="52" t="s">
-        <v>162</v>
+        <v>219</v>
       </c>
       <c r="F51" s="53"/>
     </row>
     <row r="52" spans="2:6">
       <c r="B52" s="60"/>
       <c r="C52" s="51"/>
-      <c r="D52" s="66" t="s">
+      <c r="D52" s="52"/>
+      <c r="E52" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="F52" s="53"/>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="60"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="E52" s="52"/>
-      <c r="F52" s="53"/>
-    </row>
-    <row r="53" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B53" s="60"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55" t="s">
+      <c r="E53" s="52"/>
+      <c r="F53" s="53"/>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B54" s="60"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="F53" s="56"/>
-    </row>
-    <row r="54" spans="2:6">
-      <c r="B54" s="62" t="s">
+      <c r="F54" s="56"/>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="C54" s="63" t="s">
+      <c r="C55" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="D54" s="49"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="50"/>
-    </row>
-    <row r="55" spans="2:6">
-      <c r="B55" s="60"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E55" s="52"/>
-      <c r="F55" s="53"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="50"/>
     </row>
     <row r="56" spans="2:6">
       <c r="B56" s="60"/>
       <c r="C56" s="51"/>
-      <c r="D56" s="52"/>
-      <c r="E56" s="52" t="s">
-        <v>169</v>
-      </c>
+      <c r="D56" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E56" s="52"/>
       <c r="F56" s="53"/>
     </row>
     <row r="57" spans="2:6">
@@ -5754,7 +5834,7 @@
       <c r="C57" s="51"/>
       <c r="D57" s="52"/>
       <c r="E57" s="52" t="s">
-        <v>222</v>
+        <v>169</v>
       </c>
       <c r="F57" s="53"/>
     </row>
@@ -5763,7 +5843,7 @@
       <c r="C58" s="51"/>
       <c r="D58" s="52"/>
       <c r="E58" s="52" t="s">
-        <v>171</v>
+        <v>222</v>
       </c>
       <c r="F58" s="53"/>
     </row>
@@ -5772,7 +5852,7 @@
       <c r="C59" s="51"/>
       <c r="D59" s="52"/>
       <c r="E59" s="52" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="F59" s="53"/>
     </row>
@@ -5781,7 +5861,7 @@
       <c r="C60" s="51"/>
       <c r="D60" s="52"/>
       <c r="E60" s="52" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="F60" s="53"/>
     </row>
@@ -5790,46 +5870,46 @@
       <c r="C61" s="51"/>
       <c r="D61" s="52"/>
       <c r="E61" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="F61" s="53"/>
+    </row>
+    <row r="62" spans="2:6">
+      <c r="B62" s="60"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="F61" s="53"/>
-    </row>
-    <row r="62" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B62" s="60"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55" t="s">
+      <c r="F62" s="53"/>
+    </row>
+    <row r="63" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B63" s="60"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="F62" s="56"/>
-    </row>
-    <row r="63" spans="2:6">
-      <c r="B63" s="62" t="s">
+      <c r="F63" s="56"/>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C63" s="63" t="s">
+      <c r="C64" s="63" t="s">
         <v>223</v>
       </c>
-      <c r="D63" s="49"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="50"/>
-    </row>
-    <row r="64" spans="2:6">
-      <c r="B64" s="59"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E64" s="52"/>
-      <c r="F64" s="53"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="50"/>
     </row>
     <row r="65" spans="2:6">
       <c r="B65" s="59"/>
       <c r="C65" s="51"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="52" t="s">
-        <v>164</v>
-      </c>
+      <c r="D65" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E65" s="52"/>
       <c r="F65" s="53"/>
     </row>
     <row r="66" spans="2:6">
@@ -5837,7 +5917,7 @@
       <c r="C66" s="51"/>
       <c r="D66" s="52"/>
       <c r="E66" s="52" t="s">
-        <v>224</v>
+        <v>164</v>
       </c>
       <c r="F66" s="53"/>
     </row>
@@ -5846,65 +5926,74 @@
       <c r="C67" s="51"/>
       <c r="D67" s="52"/>
       <c r="E67" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="F67" s="53"/>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="59"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="52"/>
+      <c r="E68" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="F67" s="53"/>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B68" s="59"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="55"/>
-      <c r="E68" s="55" t="s">
+      <c r="F68" s="53"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B69" s="59"/>
+      <c r="C69" s="54"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55" t="s">
         <v>226</v>
       </c>
-      <c r="F68" s="56"/>
-    </row>
-    <row r="69" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B69" s="58" t="s">
+      <c r="F69" s="56"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B70" s="58" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="70" spans="2:6">
-      <c r="B70" s="59"/>
-      <c r="C70" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="50"/>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" s="59"/>
-      <c r="C71" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="D71" s="52"/>
-      <c r="E71" s="52"/>
-      <c r="F71" s="53"/>
+      <c r="C71" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" s="49"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="50"/>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" s="59"/>
       <c r="C72" s="51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D72" s="52"/>
       <c r="E72" s="52"/>
       <c r="F72" s="53"/>
     </row>
-    <row r="73" spans="2:6" ht="15.75" thickBot="1">
+    <row r="73" spans="2:6">
       <c r="B73" s="59"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="55"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="56"/>
-    </row>
-    <row r="74" spans="2:6">
-      <c r="B74" s="58" t="s">
+      <c r="C73" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="F73" s="53"/>
+    </row>
+    <row r="74" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B74" s="59"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="56"/>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="79" spans="2:6">
-      <c r="B79" s="59"/>
+    <row r="80" spans="2:6">
+      <c r="B80" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5917,7 +6006,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A20" sqref="A20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6093,10 +6182,456 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="57" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="B2" s="71" t="s">
+        <v>248</v>
+      </c>
+      <c r="L2" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="M2" s="69"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="C3" s="73" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="C4" s="73" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="73"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73"/>
+      <c r="S7" s="73"/>
+      <c r="T7" s="73"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="73"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="73"/>
+      <c r="T10" s="73"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="73"/>
+      <c r="R11" s="73"/>
+      <c r="S11" s="73"/>
+      <c r="T11" s="73"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="73"/>
+      <c r="T12" s="73"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="73"/>
+      <c r="R13" s="73"/>
+      <c r="S13" s="73"/>
+      <c r="T13" s="73"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="B14" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="L14" s="72" t="s">
+        <v>251</v>
+      </c>
+      <c r="M14" s="72"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="73"/>
+      <c r="S15" s="73"/>
+      <c r="T15" s="73"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="73"/>
+      <c r="R16" s="73"/>
+      <c r="S16" s="73"/>
+      <c r="T16" s="73"/>
+    </row>
+    <row r="17" spans="3:20">
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="73"/>
+      <c r="R17" s="73"/>
+      <c r="S17" s="73"/>
+      <c r="T17" s="73"/>
+    </row>
+    <row r="18" spans="3:20">
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="73"/>
+      <c r="Q18" s="73"/>
+      <c r="R18" s="73"/>
+      <c r="S18" s="73"/>
+      <c r="T18" s="73"/>
+    </row>
+    <row r="19" spans="3:20">
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="73"/>
+      <c r="Q19" s="73"/>
+      <c r="R19" s="73"/>
+      <c r="S19" s="73"/>
+      <c r="T19" s="73"/>
+    </row>
+    <row r="20" spans="3:20">
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="73"/>
+      <c r="R20" s="73"/>
+      <c r="S20" s="73"/>
+      <c r="T20" s="73"/>
+    </row>
+    <row r="21" spans="3:20">
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="73"/>
+      <c r="Q21" s="73"/>
+      <c r="R21" s="73"/>
+      <c r="S21" s="73"/>
+      <c r="T21" s="73"/>
+    </row>
+    <row r="22" spans="3:20">
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="73"/>
+      <c r="P22" s="73"/>
+      <c r="Q22" s="73"/>
+      <c r="R22" s="73"/>
+      <c r="S22" s="73"/>
+      <c r="T22" s="73"/>
+    </row>
+    <row r="23" spans="3:20">
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="73"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="73"/>
+      <c r="O23" s="73"/>
+      <c r="P23" s="73"/>
+      <c r="Q23" s="73"/>
+      <c r="R23" s="73"/>
+      <c r="S23" s="73"/>
+      <c r="T23" s="73"/>
+    </row>
+    <row r="24" spans="3:20">
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="73"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="73"/>
+      <c r="S24" s="73"/>
+      <c r="T24" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
@@ -6129,13 +6664,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -6143,66 +6678,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="70" t="s">
+      <c r="K2" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="72"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="78"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="70" t="s">
+      <c r="Q2" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="72"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="78"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="79" t="s">
+      <c r="V2" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="80"/>
-      <c r="X2" s="80"/>
-      <c r="Y2" s="81"/>
+      <c r="W2" s="86"/>
+      <c r="X2" s="86"/>
+      <c r="Y2" s="87"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="82" t="s">
+      <c r="AA2" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="83"/>
-      <c r="AC2" s="83"/>
-      <c r="AD2" s="83"/>
-      <c r="AE2" s="83"/>
-      <c r="AF2" s="83"/>
-      <c r="AG2" s="84"/>
+      <c r="AB2" s="89"/>
+      <c r="AC2" s="89"/>
+      <c r="AD2" s="89"/>
+      <c r="AE2" s="89"/>
+      <c r="AF2" s="89"/>
+      <c r="AG2" s="90"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="79" t="s">
+      <c r="AI2" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="80"/>
-      <c r="AK2" s="80"/>
-      <c r="AL2" s="80"/>
-      <c r="AM2" s="80"/>
-      <c r="AN2" s="80"/>
-      <c r="AO2" s="80"/>
-      <c r="AP2" s="80"/>
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="86"/>
+      <c r="AL2" s="86"/>
+      <c r="AM2" s="86"/>
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="86"/>
+      <c r="AP2" s="86"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="91" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -6229,12 +6764,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="76"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update Bs-Rating, Product-Item Component. Done WishList Component (Membership Module)
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="253">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -1030,6 +1030,9 @@
   </si>
   <si>
     <t>profile (general page)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1371,6 +1374,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1775,8 +1784,38 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1797,36 +1836,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2960,13 +2969,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -2974,51 +2983,51 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="85" t="s">
+      <c r="K2" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="87"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="80"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="85" t="s">
+      <c r="Q2" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="87"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="80"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="77" t="s">
+      <c r="V2" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="79"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="89"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="80" t="s">
+      <c r="AA2" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="81"/>
-      <c r="AC2" s="81"/>
-      <c r="AD2" s="81"/>
-      <c r="AE2" s="81"/>
-      <c r="AF2" s="81"/>
-      <c r="AG2" s="82"/>
+      <c r="AB2" s="91"/>
+      <c r="AC2" s="91"/>
+      <c r="AD2" s="91"/>
+      <c r="AE2" s="91"/>
+      <c r="AF2" s="91"/>
+      <c r="AG2" s="92"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="77" t="s">
+      <c r="AI2" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="78"/>
-      <c r="AK2" s="78"/>
-      <c r="AL2" s="78"/>
-      <c r="AM2" s="78"/>
-      <c r="AN2" s="78"/>
-      <c r="AO2" s="78"/>
-      <c r="AP2" s="78"/>
+      <c r="AJ2" s="88"/>
+      <c r="AK2" s="88"/>
+      <c r="AL2" s="88"/>
+      <c r="AM2" s="88"/>
+      <c r="AN2" s="88"/>
+      <c r="AO2" s="88"/>
+      <c r="AP2" s="88"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="83" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="95" t="s">
@@ -3060,7 +3069,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="91"/>
+      <c r="B4" s="84"/>
       <c r="C4" s="94"/>
       <c r="D4" s="94"/>
       <c r="E4" s="94"/>
@@ -4200,41 +4209,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="86" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76" t="s">
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="76"/>
-      <c r="AB1" s="76"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="86"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -4242,66 +4251,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="85" t="s">
+      <c r="K2" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="87"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="80"/>
       <c r="P2" s="68"/>
-      <c r="Q2" s="85" t="s">
+      <c r="Q2" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="87"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="80"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="77" t="s">
+      <c r="V2" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="78"/>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="79"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
+      <c r="Y2" s="89"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="80" t="s">
+      <c r="AA2" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="81"/>
-      <c r="AC2" s="81"/>
-      <c r="AD2" s="81"/>
-      <c r="AE2" s="81"/>
-      <c r="AF2" s="81"/>
-      <c r="AG2" s="82"/>
+      <c r="AB2" s="91"/>
+      <c r="AC2" s="91"/>
+      <c r="AD2" s="91"/>
+      <c r="AE2" s="91"/>
+      <c r="AF2" s="91"/>
+      <c r="AG2" s="92"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="77" t="s">
+      <c r="AI2" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="78"/>
-      <c r="AK2" s="78"/>
-      <c r="AL2" s="78"/>
-      <c r="AM2" s="78"/>
-      <c r="AN2" s="78"/>
-      <c r="AO2" s="78"/>
-      <c r="AP2" s="78"/>
+      <c r="AJ2" s="88"/>
+      <c r="AK2" s="88"/>
+      <c r="AL2" s="88"/>
+      <c r="AM2" s="88"/>
+      <c r="AN2" s="88"/>
+      <c r="AO2" s="88"/>
+      <c r="AP2" s="88"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="76" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -4328,12 +4337,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="91"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
       <c r="H4" s="16">
         <v>1</v>
       </c>
@@ -6208,6 +6217,11 @@
     <row r="31" spans="2:52" ht="30" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:AB1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
@@ -6217,11 +6231,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:AB1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AI2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="BA5:BO30">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -6410,8 +6419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6871,10 +6880,13 @@
       <c r="B35" s="60"/>
       <c r="C35" s="51"/>
       <c r="D35" s="52"/>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="74" t="s">
         <v>200</v>
       </c>
-      <c r="F35" s="53"/>
+      <c r="F35" s="75"/>
+      <c r="G35" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="36" spans="2:7">
       <c r="B36" s="60"/>
@@ -6892,10 +6904,13 @@
       <c r="B37" s="60"/>
       <c r="C37" s="51"/>
       <c r="D37" s="52"/>
-      <c r="E37" s="74" t="s">
+      <c r="E37" s="64" t="s">
         <v>251</v>
       </c>
-      <c r="F37" s="75"/>
+      <c r="F37" s="65"/>
+      <c r="G37" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="60"/>
@@ -6929,33 +6944,45 @@
         <v>160</v>
       </c>
       <c r="F40" s="65"/>
+      <c r="G40" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="41" spans="2:7">
       <c r="B41" s="60"/>
       <c r="C41" s="51"/>
       <c r="D41" s="52"/>
-      <c r="E41" s="52" t="s">
+      <c r="E41" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="F41" s="53"/>
+      <c r="F41" s="65"/>
+      <c r="G41" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="42" spans="2:7">
       <c r="B42" s="60"/>
       <c r="C42" s="51"/>
       <c r="D42" s="52"/>
-      <c r="E42" s="52" t="s">
+      <c r="E42" s="64" t="s">
         <v>166</v>
       </c>
-      <c r="F42" s="53"/>
+      <c r="F42" s="65"/>
+      <c r="G42" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="43" spans="2:7">
       <c r="B43" s="60"/>
       <c r="C43" s="51"/>
       <c r="D43" s="52"/>
-      <c r="E43" s="52" t="s">
+      <c r="E43" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="F43" s="53"/>
+      <c r="F43" s="65"/>
+      <c r="G43" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="44" spans="2:7">
       <c r="B44" s="60"/>

</xml_diff>

<commit_message>
Done Search Filter, Google Map, Review Component (Searching Module)
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="259">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -1008,12 +1008,6 @@
     <t>IBsBreadcrumb</t>
   </si>
   <si>
-    <t>Tip:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set style cho thẻ component --&gt; sử dụng  :host trong scss ví dụ như     :host {color:  grey}    </t>
-  </si>
-  <si>
     <t>CSS</t>
   </si>
   <si>
@@ -1026,20 +1020,44 @@
     <t>Application</t>
   </si>
   <si>
-    <t>Dùng    btn-lg , input-lg    để set kích thước cho các các element trong bootstrap</t>
-  </si>
-  <si>
     <t>profile (general page)</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiện phải xóa Component thủ công, chưa có xóa tự động </t>
+  </si>
+  <si>
+    <t>TIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*set style cho thẻ component --&gt; sử dụng  :host trong scss ví dụ như     :host {color:  grey}    </t>
+  </si>
+  <si>
+    <t>*Dùng    btn-lg , input-lg    để set kích thước cho các các element trong bootstrap</t>
+  </si>
+  <si>
+    <t>*Thiết kế theo giao diện mobile trước (vì khả năng bị vỡ layout ở mobile là cao nhứt )</t>
+  </si>
+  <si>
+    <t>*Có thể linh hoạt chuyển đổi giữa Bootstrap, Ngx-Bootstrap và Angular Material</t>
+  </si>
+  <si>
+    <t>*Component con nên chỉnh maximum chiều ngang.  Khi sử dụng thì set lại theo component cha</t>
+  </si>
+  <si>
+    <t>Lỗi khi dùng [(NgModel)] --&gt; thiếu FormsModule</t>
+  </si>
+  <si>
+    <t>*Tạo các border cho tất cả Thẻ khi design sẽ dễ nhìn ra layout hơn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1288,6 +1306,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1623,7 +1649,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1780,12 +1806,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1815,27 +1865,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2969,13 +2998,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -2983,66 +3012,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="78" t="s">
+      <c r="K2" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="80"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="90"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="80"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="90"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="87" t="s">
+      <c r="V2" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="88"/>
-      <c r="X2" s="88"/>
-      <c r="Y2" s="89"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="82"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="90" t="s">
+      <c r="AA2" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="91"/>
-      <c r="AC2" s="91"/>
-      <c r="AD2" s="91"/>
-      <c r="AE2" s="91"/>
-      <c r="AF2" s="91"/>
-      <c r="AG2" s="92"/>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
+      <c r="AE2" s="84"/>
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="85"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="87" t="s">
+      <c r="AI2" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="88"/>
-      <c r="AK2" s="88"/>
-      <c r="AL2" s="88"/>
-      <c r="AM2" s="88"/>
-      <c r="AN2" s="88"/>
-      <c r="AO2" s="88"/>
-      <c r="AP2" s="88"/>
+      <c r="AJ2" s="81"/>
+      <c r="AK2" s="81"/>
+      <c r="AL2" s="81"/>
+      <c r="AM2" s="81"/>
+      <c r="AN2" s="81"/>
+      <c r="AO2" s="81"/>
+      <c r="AP2" s="81"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="96" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -3069,12 +3098,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="84"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>
@@ -4187,8 +4216,8 @@
   </sheetPr>
   <dimension ref="B1:BO31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="30" customHeight="1"/>
@@ -4209,41 +4238,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86" t="s">
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="79"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -4251,66 +4280,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="78" t="s">
+      <c r="K2" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="80"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="90"/>
       <c r="P2" s="68"/>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="80"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="90"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="87" t="s">
+      <c r="V2" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="88"/>
-      <c r="X2" s="88"/>
-      <c r="Y2" s="89"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="82"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="90" t="s">
+      <c r="AA2" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="91"/>
-      <c r="AC2" s="91"/>
-      <c r="AD2" s="91"/>
-      <c r="AE2" s="91"/>
-      <c r="AF2" s="91"/>
-      <c r="AG2" s="92"/>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
+      <c r="AE2" s="84"/>
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="85"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="87" t="s">
+      <c r="AI2" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="88"/>
-      <c r="AK2" s="88"/>
-      <c r="AL2" s="88"/>
-      <c r="AM2" s="88"/>
-      <c r="AN2" s="88"/>
-      <c r="AO2" s="88"/>
-      <c r="AP2" s="88"/>
+      <c r="AJ2" s="81"/>
+      <c r="AK2" s="81"/>
+      <c r="AL2" s="81"/>
+      <c r="AM2" s="81"/>
+      <c r="AN2" s="81"/>
+      <c r="AO2" s="81"/>
+      <c r="AP2" s="81"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="86" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -4337,12 +4366,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="84"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
       <c r="H4" s="16">
         <v>1</v>
       </c>
@@ -4352,10 +4381,10 @@
       <c r="J4" s="16">
         <v>3</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="16">
         <v>4</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="68">
         <v>5</v>
       </c>
       <c r="M4" s="9">
@@ -4741,8 +4770,8 @@
       <c r="H8"/>
       <c r="I8"/>
       <c r="J8" s="16"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="18"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="68"/>
       <c r="M8" s="18"/>
       <c r="N8"/>
       <c r="O8"/>
@@ -6217,11 +6246,6 @@
     <row r="31" spans="2:52" ht="30" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:AB1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
@@ -6231,6 +6255,11 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:AB1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AI2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="BA5:BO30">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -6263,9 +6292,9 @@
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:BO4">
+  <conditionalFormatting sqref="M4:BO4">
     <cfRule type="expression" dxfId="10" priority="8">
-      <formula>L$4=period_selected</formula>
+      <formula>M$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
@@ -6280,9 +6309,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2 H5 I6:I7"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2 H5 I6:I7 K8"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2 J8"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2 N11:V11 X13:X14 M9:N9 M10:U10 W12:X12 W13 K8:M8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2 N11:V11 X13:X14 M9:N9 M10:U10 W12:X12 W13 L8:M8"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
@@ -6420,7 +6449,7 @@
   <dimension ref="A2:T79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6880,12 +6909,12 @@
       <c r="B35" s="60"/>
       <c r="C35" s="51"/>
       <c r="D35" s="52"/>
-      <c r="E35" s="74" t="s">
+      <c r="E35" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="F35" s="75"/>
+      <c r="F35" s="73"/>
       <c r="G35" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="2:7">
@@ -6905,7 +6934,7 @@
       <c r="C37" s="51"/>
       <c r="D37" s="52"/>
       <c r="E37" s="64" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F37" s="65"/>
       <c r="G37" t="s">
@@ -7031,7 +7060,7 @@
       </c>
       <c r="F48" s="53"/>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:7">
       <c r="B49" s="60"/>
       <c r="C49" s="51"/>
       <c r="D49" s="52"/>
@@ -7040,7 +7069,7 @@
       </c>
       <c r="F49" s="53"/>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:7">
       <c r="B50" s="60"/>
       <c r="C50" s="51"/>
       <c r="D50" s="52"/>
@@ -7049,7 +7078,7 @@
       </c>
       <c r="F50" s="53"/>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:7">
       <c r="B51" s="60"/>
       <c r="C51" s="51"/>
       <c r="D51" s="52"/>
@@ -7058,7 +7087,7 @@
       </c>
       <c r="F51" s="53"/>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:7">
       <c r="B52" s="60"/>
       <c r="C52" s="51"/>
       <c r="D52" s="66" t="s">
@@ -7067,7 +7096,7 @@
       <c r="E52" s="52"/>
       <c r="F52" s="53"/>
     </row>
-    <row r="53" spans="2:6" ht="15.75" thickBot="1">
+    <row r="53" spans="2:7" ht="15.75" thickBot="1">
       <c r="B53" s="60"/>
       <c r="C53" s="54"/>
       <c r="D53" s="55"/>
@@ -7076,7 +7105,7 @@
       </c>
       <c r="F53" s="56"/>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:7">
       <c r="B54" s="62" t="s">
         <v>231</v>
       </c>
@@ -7087,7 +7116,7 @@
       <c r="E54" s="49"/>
       <c r="F54" s="50"/>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:7">
       <c r="B55" s="60"/>
       <c r="C55" s="51"/>
       <c r="D55" s="66" t="s">
@@ -7096,16 +7125,19 @@
       <c r="E55" s="52"/>
       <c r="F55" s="53"/>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:7">
       <c r="B56" s="60"/>
       <c r="C56" s="51"/>
       <c r="D56" s="52"/>
-      <c r="E56" s="52" t="s">
+      <c r="E56" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="F56" s="53"/>
-    </row>
-    <row r="57" spans="2:6">
+      <c r="F56" s="65"/>
+      <c r="G56" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7">
       <c r="B57" s="60"/>
       <c r="C57" s="51"/>
       <c r="D57" s="52"/>
@@ -7114,7 +7146,7 @@
       </c>
       <c r="F57" s="53"/>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:7">
       <c r="B58" s="60"/>
       <c r="C58" s="51"/>
       <c r="D58" s="52"/>
@@ -7123,7 +7155,7 @@
       </c>
       <c r="F58" s="53"/>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:7">
       <c r="B59" s="60"/>
       <c r="C59" s="51"/>
       <c r="D59" s="52"/>
@@ -7132,16 +7164,19 @@
       </c>
       <c r="F59" s="53"/>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="2:7">
       <c r="B60" s="60"/>
       <c r="C60" s="51"/>
       <c r="D60" s="52"/>
-      <c r="E60" s="52" t="s">
+      <c r="E60" s="64" t="s">
         <v>153</v>
       </c>
-      <c r="F60" s="53"/>
-    </row>
-    <row r="61" spans="2:6">
+      <c r="F60" s="65"/>
+      <c r="G60" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7">
       <c r="B61" s="60"/>
       <c r="C61" s="51"/>
       <c r="D61" s="52"/>
@@ -7150,16 +7185,19 @@
       </c>
       <c r="F61" s="53"/>
     </row>
-    <row r="62" spans="2:6" ht="15.75" thickBot="1">
+    <row r="62" spans="2:7" ht="15.75" thickBot="1">
       <c r="B62" s="60"/>
       <c r="C62" s="54"/>
       <c r="D62" s="55"/>
-      <c r="E62" s="55" t="s">
+      <c r="E62" s="64" t="s">
         <v>159</v>
       </c>
-      <c r="F62" s="56"/>
-    </row>
-    <row r="63" spans="2:6">
+      <c r="F62" s="65"/>
+      <c r="G62" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7">
       <c r="B63" s="62" t="s">
         <v>232</v>
       </c>
@@ -7170,7 +7208,7 @@
       <c r="E63" s="49"/>
       <c r="F63" s="50"/>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:7">
       <c r="B64" s="59"/>
       <c r="C64" s="51"/>
       <c r="D64" s="66" t="s">
@@ -7455,445 +7493,495 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="57" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="B2" s="76" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="B2" s="71" t="s">
+      <c r="L2" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="L2" s="69" t="s">
-        <v>248</v>
-      </c>
       <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="71" t="s">
+        <v>252</v>
+      </c>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57" t="s">
+        <v>250</v>
+      </c>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="C4" s="71" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="C5" s="71" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="C6" s="78" t="s">
+        <v>255</v>
+      </c>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="C7" s="78" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="71"/>
+      <c r="S7" s="71"/>
+      <c r="T7" s="71"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="C8" s="78" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="71"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="71"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="71"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="71"/>
+      <c r="S11" s="71"/>
+      <c r="T11" s="71"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="71"/>
+      <c r="T12" s="71"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="71"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="71"/>
+      <c r="Q13" s="71"/>
+      <c r="R13" s="71"/>
+      <c r="S13" s="71"/>
+      <c r="T13" s="71"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="B14" s="77" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="C4" s="73" t="s">
-        <v>250</v>
-      </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="S6" s="73"/>
-      <c r="T6" s="73"/>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="73"/>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="73"/>
-      <c r="T8" s="73"/>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="73"/>
-      <c r="T10" s="73"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="73"/>
-      <c r="T11" s="73"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="73"/>
-      <c r="O12" s="73"/>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="73"/>
-      <c r="S12" s="73"/>
-      <c r="T12" s="73"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
-      <c r="O13" s="73"/>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="73"/>
-      <c r="R13" s="73"/>
-      <c r="S13" s="73"/>
-      <c r="T13" s="73"/>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="B14" s="70" t="s">
+      <c r="L14" s="75" t="s">
         <v>247</v>
       </c>
-      <c r="L14" s="72" t="s">
-        <v>249</v>
-      </c>
-      <c r="M14" s="72"/>
+      <c r="M14" s="70"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="73"/>
-      <c r="Q15" s="73"/>
-      <c r="R15" s="73"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="73"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57" t="s">
+        <v>257</v>
+      </c>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
     </row>
     <row r="17" spans="3:20">
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="73"/>
-      <c r="O17" s="73"/>
-      <c r="P17" s="73"/>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="73"/>
-      <c r="S17" s="73"/>
-      <c r="T17" s="73"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
     </row>
     <row r="18" spans="3:20">
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="73"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="73"/>
-      <c r="Q18" s="73"/>
-      <c r="R18" s="73"/>
-      <c r="S18" s="73"/>
-      <c r="T18" s="73"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="71"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="71"/>
+      <c r="P18" s="71"/>
+      <c r="Q18" s="71"/>
+      <c r="R18" s="71"/>
+      <c r="S18" s="71"/>
+      <c r="T18" s="71"/>
     </row>
     <row r="19" spans="3:20">
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="73"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="73"/>
-      <c r="Q19" s="73"/>
-      <c r="R19" s="73"/>
-      <c r="S19" s="73"/>
-      <c r="T19" s="73"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="71"/>
+      <c r="N19" s="71"/>
+      <c r="O19" s="71"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="71"/>
+      <c r="R19" s="71"/>
+      <c r="S19" s="71"/>
+      <c r="T19" s="71"/>
     </row>
     <row r="20" spans="3:20">
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
-      <c r="N20" s="73"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="73"/>
-      <c r="Q20" s="73"/>
-      <c r="R20" s="73"/>
-      <c r="S20" s="73"/>
-      <c r="T20" s="73"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="71"/>
+      <c r="Q20" s="71"/>
+      <c r="R20" s="71"/>
+      <c r="S20" s="71"/>
+      <c r="T20" s="71"/>
     </row>
     <row r="21" spans="3:20">
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="73"/>
-      <c r="O21" s="73"/>
-      <c r="P21" s="73"/>
-      <c r="Q21" s="73"/>
-      <c r="R21" s="73"/>
-      <c r="S21" s="73"/>
-      <c r="T21" s="73"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="71"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="71"/>
+      <c r="T21" s="71"/>
     </row>
     <row r="22" spans="3:20">
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
-      <c r="O22" s="73"/>
-      <c r="P22" s="73"/>
-      <c r="Q22" s="73"/>
-      <c r="R22" s="73"/>
-      <c r="S22" s="73"/>
-      <c r="T22" s="73"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="71"/>
+      <c r="Q22" s="71"/>
+      <c r="R22" s="71"/>
+      <c r="S22" s="71"/>
+      <c r="T22" s="71"/>
     </row>
     <row r="23" spans="3:20">
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="73"/>
-      <c r="O23" s="73"/>
-      <c r="P23" s="73"/>
-      <c r="Q23" s="73"/>
-      <c r="R23" s="73"/>
-      <c r="S23" s="73"/>
-      <c r="T23" s="73"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="71"/>
+      <c r="Q23" s="71"/>
+      <c r="R23" s="71"/>
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
     </row>
     <row r="24" spans="3:20">
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="73"/>
-      <c r="N24" s="73"/>
-      <c r="O24" s="73"/>
-      <c r="P24" s="73"/>
-      <c r="Q24" s="73"/>
-      <c r="R24" s="73"/>
-      <c r="S24" s="73"/>
-      <c r="T24" s="73"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="71"/>
+      <c r="Q24" s="71"/>
+      <c r="R24" s="71"/>
+      <c r="S24" s="71"/>
+      <c r="T24" s="71"/>
+    </row>
+    <row r="25" spans="3:20">
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="71"/>
+      <c r="Q25" s="71"/>
+      <c r="R25" s="71"/>
+      <c r="S25" s="71"/>
+      <c r="T25" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done Search Filter, Search Product, Product Detail, Similar Product Component (Searching Component)
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="261">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -1051,6 +1051,12 @@
   </si>
   <si>
     <t>*Tạo các border cho tất cả Thẻ khi design sẽ dễ nhìn ra layout hơn</t>
+  </si>
+  <si>
+    <t>Giống Review</t>
+  </si>
+  <si>
+    <t>simiar-product</t>
   </si>
 </sst>
 </file>
@@ -1815,27 +1821,6 @@
     <xf numFmtId="0" fontId="32" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1865,6 +1850,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2998,13 +3004,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -3012,51 +3018,51 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="88" t="s">
+      <c r="K2" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="90"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="83"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="88" t="s">
+      <c r="Q2" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="90"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="83"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="80" t="s">
+      <c r="V2" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="81"/>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="82"/>
+      <c r="W2" s="91"/>
+      <c r="X2" s="91"/>
+      <c r="Y2" s="92"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="83" t="s">
+      <c r="AA2" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="85"/>
+      <c r="AB2" s="94"/>
+      <c r="AC2" s="94"/>
+      <c r="AD2" s="94"/>
+      <c r="AE2" s="94"/>
+      <c r="AF2" s="94"/>
+      <c r="AG2" s="95"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="80" t="s">
+      <c r="AI2" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="81"/>
-      <c r="AK2" s="81"/>
-      <c r="AL2" s="81"/>
-      <c r="AM2" s="81"/>
-      <c r="AN2" s="81"/>
-      <c r="AO2" s="81"/>
-      <c r="AP2" s="81"/>
+      <c r="AJ2" s="91"/>
+      <c r="AK2" s="91"/>
+      <c r="AL2" s="91"/>
+      <c r="AM2" s="91"/>
+      <c r="AN2" s="91"/>
+      <c r="AO2" s="91"/>
+      <c r="AP2" s="91"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="86" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="98" t="s">
@@ -3098,7 +3104,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="94"/>
+      <c r="B4" s="87"/>
       <c r="C4" s="97"/>
       <c r="D4" s="97"/>
       <c r="E4" s="97"/>
@@ -4217,7 +4223,7 @@
   <dimension ref="B1:BO31"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="30" customHeight="1"/>
@@ -4238,41 +4244,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79" t="s">
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="79"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="89"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+      <c r="AA1" s="89"/>
+      <c r="AB1" s="89"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -4280,66 +4286,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="88" t="s">
+      <c r="K2" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="90"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="83"/>
       <c r="P2" s="68"/>
-      <c r="Q2" s="88" t="s">
+      <c r="Q2" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="90"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="83"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="80" t="s">
+      <c r="V2" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="81"/>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="82"/>
+      <c r="W2" s="91"/>
+      <c r="X2" s="91"/>
+      <c r="Y2" s="92"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="83" t="s">
+      <c r="AA2" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="85"/>
+      <c r="AB2" s="94"/>
+      <c r="AC2" s="94"/>
+      <c r="AD2" s="94"/>
+      <c r="AE2" s="94"/>
+      <c r="AF2" s="94"/>
+      <c r="AG2" s="95"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="80" t="s">
+      <c r="AI2" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="81"/>
-      <c r="AK2" s="81"/>
-      <c r="AL2" s="81"/>
-      <c r="AM2" s="81"/>
-      <c r="AN2" s="81"/>
-      <c r="AO2" s="81"/>
-      <c r="AP2" s="81"/>
+      <c r="AJ2" s="91"/>
+      <c r="AK2" s="91"/>
+      <c r="AL2" s="91"/>
+      <c r="AM2" s="91"/>
+      <c r="AN2" s="91"/>
+      <c r="AO2" s="91"/>
+      <c r="AP2" s="91"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="95" t="s">
+      <c r="D3" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="86" t="s">
+      <c r="G3" s="79" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -4366,12 +4372,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="94"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
       <c r="H4" s="16">
         <v>1</v>
       </c>
@@ -6246,6 +6252,11 @@
     <row r="31" spans="2:52" ht="30" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:AB1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
@@ -6255,11 +6266,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:AB1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AI2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="BA5:BO30">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -6446,10 +6452,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T79"/>
+  <dimension ref="A2:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7060,7 +7066,7 @@
       </c>
       <c r="F48" s="53"/>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:8">
       <c r="B49" s="60"/>
       <c r="C49" s="51"/>
       <c r="D49" s="52"/>
@@ -7069,7 +7075,7 @@
       </c>
       <c r="F49" s="53"/>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:8">
       <c r="B50" s="60"/>
       <c r="C50" s="51"/>
       <c r="D50" s="52"/>
@@ -7078,7 +7084,7 @@
       </c>
       <c r="F50" s="53"/>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:8">
       <c r="B51" s="60"/>
       <c r="C51" s="51"/>
       <c r="D51" s="52"/>
@@ -7087,7 +7093,7 @@
       </c>
       <c r="F51" s="53"/>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="2:8">
       <c r="B52" s="60"/>
       <c r="C52" s="51"/>
       <c r="D52" s="66" t="s">
@@ -7096,7 +7102,7 @@
       <c r="E52" s="52"/>
       <c r="F52" s="53"/>
     </row>
-    <row r="53" spans="2:7" ht="15.75" thickBot="1">
+    <row r="53" spans="2:8" ht="15.75" thickBot="1">
       <c r="B53" s="60"/>
       <c r="C53" s="54"/>
       <c r="D53" s="55"/>
@@ -7105,7 +7111,7 @@
       </c>
       <c r="F53" s="56"/>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="2:8">
       <c r="B54" s="62" t="s">
         <v>231</v>
       </c>
@@ -7116,7 +7122,7 @@
       <c r="E54" s="49"/>
       <c r="F54" s="50"/>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:8">
       <c r="B55" s="60"/>
       <c r="C55" s="51"/>
       <c r="D55" s="66" t="s">
@@ -7125,7 +7131,7 @@
       <c r="E55" s="52"/>
       <c r="F55" s="53"/>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:8">
       <c r="B56" s="60"/>
       <c r="C56" s="51"/>
       <c r="D56" s="52"/>
@@ -7137,93 +7143,108 @@
         <v>242</v>
       </c>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:8">
       <c r="B57" s="60"/>
       <c r="C57" s="51"/>
       <c r="D57" s="52"/>
-      <c r="E57" s="52" t="s">
+      <c r="E57" s="64" t="s">
         <v>221</v>
       </c>
-      <c r="F57" s="53"/>
-    </row>
-    <row r="58" spans="2:7">
+      <c r="F57" s="65"/>
+      <c r="G57" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
       <c r="B58" s="60"/>
       <c r="C58" s="51"/>
       <c r="D58" s="52"/>
-      <c r="E58" s="52" t="s">
+      <c r="E58" s="64" t="s">
         <v>171</v>
       </c>
-      <c r="F58" s="53"/>
-    </row>
-    <row r="59" spans="2:7">
+      <c r="F58" s="65"/>
+      <c r="G58" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
       <c r="B59" s="60"/>
       <c r="C59" s="51"/>
       <c r="D59" s="52"/>
-      <c r="E59" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="F59" s="53"/>
-    </row>
-    <row r="60" spans="2:7">
+      <c r="E59" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="F59" s="65"/>
+      <c r="G59" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8">
       <c r="B60" s="60"/>
       <c r="C60" s="51"/>
       <c r="D60" s="52"/>
-      <c r="E60" s="64" t="s">
-        <v>153</v>
-      </c>
-      <c r="F60" s="65"/>
-      <c r="G60" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7">
+      <c r="E60" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="F60" s="53"/>
+    </row>
+    <row r="61" spans="2:8">
       <c r="B61" s="60"/>
       <c r="C61" s="51"/>
       <c r="D61" s="52"/>
-      <c r="E61" s="52" t="s">
+      <c r="E61" s="64" t="s">
+        <v>153</v>
+      </c>
+      <c r="F61" s="65"/>
+      <c r="G61" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="60"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="72" t="s">
         <v>158</v>
       </c>
-      <c r="F61" s="53"/>
-    </row>
-    <row r="62" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B62" s="60"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="64" t="s">
+      <c r="F62" s="73"/>
+      <c r="G62" t="s">
+        <v>249</v>
+      </c>
+      <c r="H62" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B63" s="60"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="64" t="s">
         <v>159</v>
       </c>
-      <c r="F62" s="65"/>
-      <c r="G62" t="s">
+      <c r="F63" s="65"/>
+      <c r="G63" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="63" spans="2:7">
-      <c r="B63" s="62" t="s">
+    <row r="64" spans="2:8">
+      <c r="B64" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="C63" s="63" t="s">
+      <c r="C64" s="63" t="s">
         <v>222</v>
       </c>
-      <c r="D63" s="49"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="50"/>
-    </row>
-    <row r="64" spans="2:7">
-      <c r="B64" s="59"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="E64" s="52"/>
-      <c r="F64" s="53"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="50"/>
     </row>
     <row r="65" spans="2:6">
       <c r="B65" s="59"/>
       <c r="C65" s="51"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="52" t="s">
-        <v>164</v>
-      </c>
+      <c r="D65" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="E65" s="52"/>
       <c r="F65" s="53"/>
     </row>
     <row r="66" spans="2:6">
@@ -7231,7 +7252,7 @@
       <c r="C66" s="51"/>
       <c r="D66" s="52"/>
       <c r="E66" s="52" t="s">
-        <v>223</v>
+        <v>164</v>
       </c>
       <c r="F66" s="53"/>
     </row>
@@ -7240,65 +7261,74 @@
       <c r="C67" s="51"/>
       <c r="D67" s="52"/>
       <c r="E67" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="F67" s="53"/>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="59"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="52"/>
+      <c r="E68" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="F67" s="53"/>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B68" s="59"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="55"/>
-      <c r="E68" s="55" t="s">
+      <c r="F68" s="53"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B69" s="59"/>
+      <c r="C69" s="54"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="F68" s="56"/>
-    </row>
-    <row r="69" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B69" s="58" t="s">
+      <c r="F69" s="56"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B70" s="58" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="70" spans="2:6">
-      <c r="B70" s="59"/>
-      <c r="C70" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="50"/>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" s="59"/>
-      <c r="C71" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="D71" s="52"/>
-      <c r="E71" s="52"/>
-      <c r="F71" s="53"/>
+      <c r="C71" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" s="49"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="50"/>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" s="59"/>
       <c r="C72" s="51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D72" s="52"/>
       <c r="E72" s="52"/>
       <c r="F72" s="53"/>
     </row>
-    <row r="73" spans="2:6" ht="15.75" thickBot="1">
+    <row r="73" spans="2:6">
       <c r="B73" s="59"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="55"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="56"/>
-    </row>
-    <row r="74" spans="2:6">
-      <c r="B74" s="58" t="s">
+      <c r="C73" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="D73" s="52"/>
+      <c r="E73" s="52"/>
+      <c r="F73" s="53"/>
+    </row>
+    <row r="74" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B74" s="59"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="56"/>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="58" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="79" spans="2:6">
-      <c r="B79" s="59"/>
+    <row r="80" spans="2:6">
+      <c r="B80" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add note in excel file ts
</commit_message>
<xml_diff>
--- a/Document/TTTN_Tuan_Phuong.xlsx
+++ b/Document/TTTN_Tuan_Phuong.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="258">
   <si>
     <t>Đạt môn học</t>
   </si>
@@ -1825,72 +1825,72 @@
     <xf numFmtId="0" fontId="33" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="20"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="17">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -3016,13 +3016,13 @@
       <c r="G1" s="21"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
       <c r="G2" s="20" t="s">
         <v>45</v>
       </c>
@@ -3030,66 +3030,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="86" t="s">
+      <c r="K2" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="88"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="84"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="86" t="s">
+      <c r="Q2" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="88"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="84"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="78" t="s">
+      <c r="V2" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="80"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="93"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="81" t="s">
+      <c r="AA2" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82"/>
-      <c r="AE2" s="82"/>
-      <c r="AF2" s="82"/>
-      <c r="AG2" s="83"/>
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="95"/>
+      <c r="AD2" s="95"/>
+      <c r="AE2" s="95"/>
+      <c r="AF2" s="95"/>
+      <c r="AG2" s="96"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="78" t="s">
+      <c r="AI2" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="79"/>
-      <c r="AK2" s="79"/>
-      <c r="AL2" s="79"/>
-      <c r="AM2" s="79"/>
-      <c r="AN2" s="79"/>
-      <c r="AO2" s="79"/>
-      <c r="AP2" s="79"/>
+      <c r="AJ2" s="92"/>
+      <c r="AK2" s="92"/>
+      <c r="AL2" s="92"/>
+      <c r="AM2" s="92"/>
+      <c r="AN2" s="92"/>
+      <c r="AO2" s="92"/>
+      <c r="AP2" s="92"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="96" t="s">
+      <c r="F3" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="94" t="s">
+      <c r="G3" s="97" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -3116,12 +3116,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1">
-      <c r="B4" s="92"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
       <c r="H4" s="9">
         <v>1</v>
       </c>
@@ -4256,41 +4256,41 @@
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
       <c r="F1" s="39"/>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77" t="s">
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="90"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="90"/>
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
       <c r="G2" s="40" t="s">
         <v>45</v>
       </c>
@@ -4298,66 +4298,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="18"/>
-      <c r="K2" s="86" t="s">
+      <c r="K2" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="88"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="84"/>
       <c r="P2" s="68"/>
-      <c r="Q2" s="86" t="s">
+      <c r="Q2" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="88"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="84"/>
       <c r="U2" s="16"/>
-      <c r="V2" s="78" t="s">
+      <c r="V2" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="80"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="93"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="81" t="s">
+      <c r="AA2" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="82"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="82"/>
-      <c r="AE2" s="82"/>
-      <c r="AF2" s="82"/>
-      <c r="AG2" s="83"/>
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="95"/>
+      <c r="AD2" s="95"/>
+      <c r="AE2" s="95"/>
+      <c r="AF2" s="95"/>
+      <c r="AG2" s="96"/>
       <c r="AH2" s="14"/>
-      <c r="AI2" s="78" t="s">
+      <c r="AI2" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="AJ2" s="79"/>
-      <c r="AK2" s="79"/>
-      <c r="AL2" s="79"/>
-      <c r="AM2" s="79"/>
-      <c r="AN2" s="79"/>
-      <c r="AO2" s="79"/>
-      <c r="AP2" s="79"/>
+      <c r="AJ2" s="92"/>
+      <c r="AK2" s="92"/>
+      <c r="AL2" s="92"/>
+      <c r="AM2" s="92"/>
+      <c r="AN2" s="92"/>
+      <c r="AO2" s="92"/>
+      <c r="AP2" s="92"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="93" t="s">
+      <c r="D3" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="80" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -4384,12 +4384,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="92"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
       <c r="H4" s="16">
         <v>1</v>
       </c>
@@ -6264,6 +6264,11 @@
     <row r="31" spans="2:52" ht="30" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G1:N1"/>
+    <mergeCell ref="O1:AB1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AI2:AP2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:T2"/>
@@ -6273,11 +6278,6 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G1:N1"/>
-    <mergeCell ref="O1:AB1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AI2:AP2"/>
   </mergeCells>
   <conditionalFormatting sqref="BA5:BO30">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -6466,8 +6466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7058,10 +7058,13 @@
       <c r="B48" s="60"/>
       <c r="C48" s="51"/>
       <c r="D48" s="52"/>
-      <c r="E48" s="52" t="s">
+      <c r="E48" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="F48" s="53"/>
+      <c r="F48" s="65"/>
+      <c r="G48" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="49" spans="2:7">
       <c r="B49" s="60"/>
@@ -7519,7 +7522,7 @@
       <c r="C3" s="73" t="s">
         <v>245</v>
       </c>
-      <c r="Q3" s="97" t="s">
+      <c r="Q3" s="77" t="s">
         <v>253</v>
       </c>
     </row>
@@ -7663,7 +7666,7 @@
       <c r="J10" s="73"/>
       <c r="K10" s="73"/>
       <c r="P10" s="73"/>
-      <c r="Q10" s="99"/>
+      <c r="Q10" s="79"/>
       <c r="R10" s="73"/>
       <c r="S10" s="73"/>
       <c r="T10" s="73"/>
@@ -7683,7 +7686,7 @@
       <c r="J11" s="73"/>
       <c r="K11" s="73"/>
       <c r="P11" s="73"/>
-      <c r="Q11" s="99"/>
+      <c r="Q11" s="79"/>
       <c r="R11" s="73"/>
       <c r="S11" s="73"/>
       <c r="T11" s="73"/>
@@ -7703,7 +7706,7 @@
       <c r="J12" s="73"/>
       <c r="K12" s="73"/>
       <c r="P12" s="73"/>
-      <c r="Q12" s="98"/>
+      <c r="Q12" s="78"/>
       <c r="V12" s="73"/>
       <c r="W12" s="73"/>
       <c r="X12" s="73"/>
@@ -7757,7 +7760,7 @@
       <c r="J16" s="73"/>
       <c r="K16" s="73"/>
       <c r="P16" s="73"/>
-      <c r="Q16" s="99"/>
+      <c r="Q16" s="79"/>
       <c r="V16" s="73"/>
       <c r="W16" s="73"/>
       <c r="X16" s="73"/>
@@ -7818,7 +7821,7 @@
       <c r="J20" s="73"/>
       <c r="K20" s="73"/>
       <c r="P20" s="73"/>
-      <c r="Q20" s="99"/>
+      <c r="Q20" s="79"/>
       <c r="R20" s="73"/>
       <c r="S20" s="73"/>
       <c r="T20" s="73"/>
@@ -7838,7 +7841,7 @@
       <c r="J21" s="73"/>
       <c r="K21" s="73"/>
       <c r="P21" s="73"/>
-      <c r="Q21" s="99"/>
+      <c r="Q21" s="79"/>
       <c r="R21" s="73"/>
       <c r="S21" s="73"/>
       <c r="T21" s="73"/>
@@ -7858,7 +7861,7 @@
       <c r="J22" s="73"/>
       <c r="K22" s="73"/>
       <c r="P22" s="73"/>
-      <c r="Q22" s="99"/>
+      <c r="Q22" s="79"/>
       <c r="R22" s="73"/>
       <c r="S22" s="73"/>
       <c r="T22" s="73"/>

</xml_diff>